<commit_message>
updeted plan vs actual ganttchart
</commit_message>
<xml_diff>
--- a/Final_Campus-Sink_Gantt Chart.xlsx
+++ b/Final_Campus-Sink_Gantt Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHRAVANI\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhira\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8751ED19-B757-4F0F-9187-DA0B60202E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3D417D-8E2F-4A51-89E8-37899030F543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="53">
   <si>
     <t>April 2025</t>
   </si>
@@ -165,12 +165,40 @@
   <si>
     <t>QA:-</t>
   </si>
+  <si>
+    <t>Actual Start Date</t>
+  </si>
+  <si>
+    <t>Actual End Date</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> VS</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,15 +210,49 @@
       <sz val="11"/>
       <color rgb="FF12355B"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF12355B"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +287,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FFF5F5F5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -329,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -357,11 +425,17 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,13 +738,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ABI35"/>
+  <dimension ref="A1:ABI64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="66" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="66" workbookViewId="0">
       <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="CN44" sqref="CN44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,7 +753,7 @@
     <col min="2" max="2" width="30" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="6" width="12" customWidth="1"/>
+    <col min="5" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="737" width="3.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -690,751 +764,751 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="22" t="s">
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="21"/>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21"/>
-      <c r="AN1" s="21"/>
-      <c r="AO1" s="21"/>
-      <c r="AP1" s="21"/>
-      <c r="AQ1" s="21"/>
-      <c r="AR1" s="23"/>
-      <c r="AS1" s="22" t="s">
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="AT1" s="21"/>
-      <c r="AU1" s="21"/>
-      <c r="AV1" s="21"/>
-      <c r="AW1" s="21"/>
-      <c r="AX1" s="21"/>
-      <c r="AY1" s="21"/>
-      <c r="AZ1" s="21"/>
-      <c r="BA1" s="21"/>
-      <c r="BB1" s="21"/>
-      <c r="BC1" s="21"/>
-      <c r="BD1" s="21"/>
-      <c r="BE1" s="21"/>
-      <c r="BF1" s="21"/>
-      <c r="BG1" s="21"/>
-      <c r="BH1" s="21"/>
-      <c r="BI1" s="21"/>
-      <c r="BJ1" s="21"/>
-      <c r="BK1" s="21"/>
-      <c r="BL1" s="21"/>
-      <c r="BM1" s="21"/>
-      <c r="BN1" s="21"/>
-      <c r="BO1" s="21"/>
-      <c r="BP1" s="21"/>
-      <c r="BQ1" s="21"/>
-      <c r="BR1" s="21"/>
-      <c r="BS1" s="21"/>
-      <c r="BT1" s="21"/>
-      <c r="BU1" s="21"/>
-      <c r="BV1" s="23"/>
-      <c r="BW1" s="22" t="s">
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="25"/>
+      <c r="AY1" s="25"/>
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="25"/>
+      <c r="BB1" s="25"/>
+      <c r="BC1" s="25"/>
+      <c r="BD1" s="25"/>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="BX1" s="21"/>
-      <c r="BY1" s="21"/>
-      <c r="BZ1" s="21"/>
-      <c r="CA1" s="21"/>
-      <c r="CB1" s="21"/>
-      <c r="CC1" s="21"/>
-      <c r="CD1" s="21"/>
-      <c r="CE1" s="21"/>
-      <c r="CF1" s="21"/>
-      <c r="CG1" s="21"/>
-      <c r="CH1" s="21"/>
-      <c r="CI1" s="21"/>
-      <c r="CJ1" s="21"/>
-      <c r="CK1" s="21"/>
-      <c r="CL1" s="21"/>
-      <c r="CM1" s="21"/>
-      <c r="CN1" s="21"/>
-      <c r="CO1" s="21"/>
-      <c r="CP1" s="21"/>
-      <c r="CQ1" s="21"/>
-      <c r="CR1" s="21"/>
-      <c r="CS1" s="21"/>
-      <c r="CT1" s="21"/>
-      <c r="CU1" s="21"/>
-      <c r="CV1" s="21"/>
-      <c r="CW1" s="21"/>
-      <c r="CX1" s="21"/>
-      <c r="CY1" s="21"/>
-      <c r="CZ1" s="21"/>
-      <c r="DA1" s="23"/>
-      <c r="DB1" s="22" t="s">
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25"/>
+      <c r="BZ1" s="25"/>
+      <c r="CA1" s="25"/>
+      <c r="CB1" s="25"/>
+      <c r="CC1" s="25"/>
+      <c r="CD1" s="25"/>
+      <c r="CE1" s="25"/>
+      <c r="CF1" s="25"/>
+      <c r="CG1" s="25"/>
+      <c r="CH1" s="25"/>
+      <c r="CI1" s="25"/>
+      <c r="CJ1" s="25"/>
+      <c r="CK1" s="25"/>
+      <c r="CL1" s="25"/>
+      <c r="CM1" s="25"/>
+      <c r="CN1" s="25"/>
+      <c r="CO1" s="25"/>
+      <c r="CP1" s="25"/>
+      <c r="CQ1" s="25"/>
+      <c r="CR1" s="25"/>
+      <c r="CS1" s="25"/>
+      <c r="CT1" s="25"/>
+      <c r="CU1" s="25"/>
+      <c r="CV1" s="25"/>
+      <c r="CW1" s="25"/>
+      <c r="CX1" s="25"/>
+      <c r="CY1" s="25"/>
+      <c r="CZ1" s="25"/>
+      <c r="DA1" s="26"/>
+      <c r="DB1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="DC1" s="21"/>
-      <c r="DD1" s="21"/>
-      <c r="DE1" s="21"/>
-      <c r="DF1" s="21"/>
-      <c r="DG1" s="21"/>
-      <c r="DH1" s="21"/>
-      <c r="DI1" s="21"/>
-      <c r="DJ1" s="21"/>
-      <c r="DK1" s="21"/>
-      <c r="DL1" s="21"/>
-      <c r="DM1" s="21"/>
-      <c r="DN1" s="21"/>
-      <c r="DO1" s="21"/>
-      <c r="DP1" s="21"/>
-      <c r="DQ1" s="21"/>
-      <c r="DR1" s="21"/>
-      <c r="DS1" s="21"/>
-      <c r="DT1" s="21"/>
-      <c r="DU1" s="21"/>
-      <c r="DV1" s="21"/>
-      <c r="DW1" s="21"/>
-      <c r="DX1" s="21"/>
-      <c r="DY1" s="21"/>
-      <c r="DZ1" s="21"/>
-      <c r="EA1" s="21"/>
-      <c r="EB1" s="21"/>
-      <c r="EC1" s="21"/>
-      <c r="ED1" s="21"/>
-      <c r="EE1" s="21"/>
-      <c r="EF1" s="23"/>
-      <c r="EG1" s="22" t="s">
+      <c r="DC1" s="25"/>
+      <c r="DD1" s="25"/>
+      <c r="DE1" s="25"/>
+      <c r="DF1" s="25"/>
+      <c r="DG1" s="25"/>
+      <c r="DH1" s="25"/>
+      <c r="DI1" s="25"/>
+      <c r="DJ1" s="25"/>
+      <c r="DK1" s="25"/>
+      <c r="DL1" s="25"/>
+      <c r="DM1" s="25"/>
+      <c r="DN1" s="25"/>
+      <c r="DO1" s="25"/>
+      <c r="DP1" s="25"/>
+      <c r="DQ1" s="25"/>
+      <c r="DR1" s="25"/>
+      <c r="DS1" s="25"/>
+      <c r="DT1" s="25"/>
+      <c r="DU1" s="25"/>
+      <c r="DV1" s="25"/>
+      <c r="DW1" s="25"/>
+      <c r="DX1" s="25"/>
+      <c r="DY1" s="25"/>
+      <c r="DZ1" s="25"/>
+      <c r="EA1" s="25"/>
+      <c r="EB1" s="25"/>
+      <c r="EC1" s="25"/>
+      <c r="ED1" s="25"/>
+      <c r="EE1" s="25"/>
+      <c r="EF1" s="26"/>
+      <c r="EG1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="EH1" s="21"/>
-      <c r="EI1" s="21"/>
-      <c r="EJ1" s="21"/>
-      <c r="EK1" s="21"/>
-      <c r="EL1" s="21"/>
-      <c r="EM1" s="21"/>
-      <c r="EN1" s="21"/>
-      <c r="EO1" s="21"/>
-      <c r="EP1" s="21"/>
-      <c r="EQ1" s="21"/>
-      <c r="ER1" s="21"/>
-      <c r="ES1" s="21"/>
-      <c r="ET1" s="21"/>
-      <c r="EU1" s="21"/>
-      <c r="EV1" s="21"/>
-      <c r="EW1" s="21"/>
-      <c r="EX1" s="21"/>
-      <c r="EY1" s="21"/>
-      <c r="EZ1" s="21"/>
-      <c r="FA1" s="21"/>
-      <c r="FB1" s="21"/>
-      <c r="FC1" s="21"/>
-      <c r="FD1" s="21"/>
-      <c r="FE1" s="21"/>
-      <c r="FF1" s="21"/>
-      <c r="FG1" s="21"/>
-      <c r="FH1" s="21"/>
-      <c r="FI1" s="21"/>
-      <c r="FJ1" s="23"/>
-      <c r="FK1" s="22" t="s">
+      <c r="EH1" s="25"/>
+      <c r="EI1" s="25"/>
+      <c r="EJ1" s="25"/>
+      <c r="EK1" s="25"/>
+      <c r="EL1" s="25"/>
+      <c r="EM1" s="25"/>
+      <c r="EN1" s="25"/>
+      <c r="EO1" s="25"/>
+      <c r="EP1" s="25"/>
+      <c r="EQ1" s="25"/>
+      <c r="ER1" s="25"/>
+      <c r="ES1" s="25"/>
+      <c r="ET1" s="25"/>
+      <c r="EU1" s="25"/>
+      <c r="EV1" s="25"/>
+      <c r="EW1" s="25"/>
+      <c r="EX1" s="25"/>
+      <c r="EY1" s="25"/>
+      <c r="EZ1" s="25"/>
+      <c r="FA1" s="25"/>
+      <c r="FB1" s="25"/>
+      <c r="FC1" s="25"/>
+      <c r="FD1" s="25"/>
+      <c r="FE1" s="25"/>
+      <c r="FF1" s="25"/>
+      <c r="FG1" s="25"/>
+      <c r="FH1" s="25"/>
+      <c r="FI1" s="25"/>
+      <c r="FJ1" s="26"/>
+      <c r="FK1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="FL1" s="21"/>
-      <c r="FM1" s="21"/>
-      <c r="FN1" s="21"/>
-      <c r="FO1" s="21"/>
-      <c r="FP1" s="21"/>
-      <c r="FQ1" s="21"/>
-      <c r="FR1" s="21"/>
-      <c r="FS1" s="21"/>
-      <c r="FT1" s="21"/>
-      <c r="FU1" s="21"/>
-      <c r="FV1" s="21"/>
-      <c r="FW1" s="21"/>
-      <c r="FX1" s="21"/>
-      <c r="FY1" s="21"/>
-      <c r="FZ1" s="21"/>
-      <c r="GA1" s="21"/>
-      <c r="GB1" s="21"/>
-      <c r="GC1" s="21"/>
-      <c r="GD1" s="21"/>
-      <c r="GE1" s="21"/>
-      <c r="GF1" s="21"/>
-      <c r="GG1" s="21"/>
-      <c r="GH1" s="21"/>
-      <c r="GI1" s="21"/>
-      <c r="GJ1" s="21"/>
-      <c r="GK1" s="21"/>
-      <c r="GL1" s="21"/>
-      <c r="GM1" s="21"/>
-      <c r="GN1" s="21"/>
-      <c r="GO1" s="23"/>
-      <c r="GP1" s="21"/>
-      <c r="GQ1" s="21"/>
-      <c r="GR1" s="21"/>
-      <c r="GS1" s="21"/>
-      <c r="GT1" s="21"/>
-      <c r="GU1" s="21"/>
-      <c r="GV1" s="21"/>
-      <c r="GW1" s="21"/>
-      <c r="GX1" s="21"/>
-      <c r="GY1" s="21"/>
-      <c r="GZ1" s="21"/>
-      <c r="HA1" s="21"/>
-      <c r="HB1" s="21"/>
-      <c r="HC1" s="21"/>
-      <c r="HD1" s="21"/>
-      <c r="HE1" s="21"/>
-      <c r="HF1" s="21"/>
-      <c r="HG1" s="21"/>
-      <c r="HH1" s="21"/>
-      <c r="HI1" s="21"/>
-      <c r="HJ1" s="21"/>
-      <c r="HK1" s="21"/>
-      <c r="HL1" s="21"/>
-      <c r="HM1" s="21"/>
-      <c r="HN1" s="21"/>
-      <c r="HO1" s="21"/>
-      <c r="HP1" s="21"/>
-      <c r="HQ1" s="21"/>
-      <c r="HR1" s="21"/>
-      <c r="HS1" s="21"/>
-      <c r="HT1" s="21"/>
-      <c r="HU1" s="21"/>
-      <c r="HV1" s="21"/>
-      <c r="HW1" s="21"/>
-      <c r="HX1" s="21"/>
-      <c r="HY1" s="21"/>
-      <c r="HZ1" s="21"/>
-      <c r="IA1" s="21"/>
-      <c r="IB1" s="21"/>
-      <c r="IC1" s="21"/>
-      <c r="ID1" s="21"/>
-      <c r="IE1" s="21"/>
-      <c r="IF1" s="21"/>
-      <c r="IG1" s="21"/>
-      <c r="IH1" s="21"/>
-      <c r="II1" s="21"/>
-      <c r="IJ1" s="21"/>
-      <c r="IK1" s="21"/>
-      <c r="IL1" s="21"/>
-      <c r="IM1" s="21"/>
-      <c r="IN1" s="21"/>
-      <c r="IO1" s="21"/>
-      <c r="IP1" s="21"/>
-      <c r="IQ1" s="21"/>
-      <c r="IR1" s="21"/>
-      <c r="IS1" s="21"/>
-      <c r="IT1" s="21"/>
-      <c r="IU1" s="21"/>
-      <c r="IV1" s="21"/>
-      <c r="IW1" s="21"/>
-      <c r="IX1" s="21"/>
-      <c r="IY1" s="21"/>
-      <c r="IZ1" s="21"/>
-      <c r="JA1" s="21"/>
-      <c r="JB1" s="21"/>
-      <c r="JC1" s="21"/>
-      <c r="JD1" s="21"/>
-      <c r="JE1" s="21"/>
-      <c r="JF1" s="21"/>
-      <c r="JG1" s="21"/>
-      <c r="JH1" s="21"/>
-      <c r="JI1" s="21"/>
-      <c r="JJ1" s="21"/>
-      <c r="JK1" s="21"/>
-      <c r="JL1" s="21"/>
-      <c r="JM1" s="21"/>
-      <c r="JN1" s="21"/>
-      <c r="JO1" s="21"/>
-      <c r="JP1" s="21"/>
-      <c r="JQ1" s="21"/>
-      <c r="JR1" s="21"/>
-      <c r="JS1" s="21"/>
-      <c r="JT1" s="21"/>
-      <c r="JU1" s="21"/>
-      <c r="JV1" s="21"/>
-      <c r="JW1" s="21"/>
-      <c r="JX1" s="21"/>
-      <c r="JY1" s="21"/>
-      <c r="JZ1" s="21"/>
-      <c r="KA1" s="21"/>
-      <c r="KB1" s="21"/>
-      <c r="KC1" s="21"/>
-      <c r="KD1" s="21"/>
-      <c r="KE1" s="21"/>
-      <c r="KF1" s="21"/>
-      <c r="KG1" s="21"/>
-      <c r="KH1" s="21"/>
-      <c r="KI1" s="21"/>
-      <c r="KJ1" s="21"/>
-      <c r="KK1" s="21"/>
-      <c r="KL1" s="21"/>
-      <c r="KM1" s="21"/>
-      <c r="KN1" s="21"/>
-      <c r="KO1" s="21"/>
-      <c r="KP1" s="21"/>
-      <c r="KQ1" s="21"/>
-      <c r="KR1" s="21"/>
-      <c r="KS1" s="21"/>
-      <c r="KT1" s="21"/>
-      <c r="KU1" s="21"/>
-      <c r="KV1" s="21"/>
-      <c r="KW1" s="21"/>
-      <c r="KX1" s="21"/>
-      <c r="KY1" s="21"/>
-      <c r="KZ1" s="21"/>
-      <c r="LA1" s="21"/>
-      <c r="LB1" s="21"/>
-      <c r="LC1" s="21"/>
-      <c r="LD1" s="21"/>
-      <c r="LE1" s="21"/>
-      <c r="LF1" s="21"/>
-      <c r="LG1" s="21"/>
-      <c r="LH1" s="21"/>
-      <c r="LI1" s="21"/>
-      <c r="LJ1" s="21"/>
-      <c r="LK1" s="21"/>
-      <c r="LL1" s="21"/>
-      <c r="LM1" s="21"/>
-      <c r="LN1" s="21"/>
-      <c r="LO1" s="21"/>
-      <c r="LP1" s="21"/>
-      <c r="LQ1" s="21"/>
-      <c r="LR1" s="21"/>
-      <c r="LS1" s="21"/>
-      <c r="LT1" s="21"/>
-      <c r="LU1" s="21"/>
-      <c r="LV1" s="21"/>
-      <c r="LW1" s="21"/>
-      <c r="LX1" s="21"/>
-      <c r="LY1" s="21"/>
-      <c r="LZ1" s="21"/>
-      <c r="MA1" s="21"/>
-      <c r="MB1" s="21"/>
-      <c r="MC1" s="21"/>
-      <c r="MD1" s="21"/>
-      <c r="ME1" s="21"/>
-      <c r="MF1" s="21"/>
-      <c r="MG1" s="21"/>
-      <c r="MH1" s="21"/>
-      <c r="MI1" s="21"/>
-      <c r="MJ1" s="21"/>
-      <c r="MK1" s="21"/>
-      <c r="ML1" s="21"/>
-      <c r="MM1" s="21"/>
-      <c r="MN1" s="21"/>
-      <c r="MO1" s="21"/>
-      <c r="MP1" s="21"/>
-      <c r="MQ1" s="21"/>
-      <c r="MR1" s="21"/>
-      <c r="MS1" s="21"/>
-      <c r="MT1" s="21"/>
-      <c r="MU1" s="21"/>
-      <c r="MV1" s="21"/>
-      <c r="MW1" s="21"/>
-      <c r="MX1" s="21"/>
-      <c r="MY1" s="21"/>
-      <c r="MZ1" s="21"/>
-      <c r="NA1" s="21"/>
-      <c r="NB1" s="21"/>
-      <c r="NC1" s="21"/>
-      <c r="ND1" s="21"/>
-      <c r="NE1" s="21"/>
-      <c r="NF1" s="21"/>
-      <c r="NG1" s="21"/>
-      <c r="NH1" s="21"/>
-      <c r="NI1" s="21"/>
-      <c r="NJ1" s="21"/>
-      <c r="NK1" s="21"/>
-      <c r="NL1" s="21"/>
-      <c r="NM1" s="21"/>
-      <c r="NN1" s="21"/>
-      <c r="NO1" s="21"/>
-      <c r="NP1" s="21"/>
-      <c r="NQ1" s="21"/>
-      <c r="NR1" s="21"/>
-      <c r="NS1" s="21"/>
-      <c r="NT1" s="21"/>
-      <c r="NU1" s="21"/>
-      <c r="NV1" s="21"/>
-      <c r="NW1" s="21"/>
-      <c r="NX1" s="21"/>
-      <c r="NY1" s="21"/>
-      <c r="NZ1" s="21"/>
-      <c r="OA1" s="21"/>
-      <c r="OB1" s="21"/>
-      <c r="OC1" s="21"/>
-      <c r="OD1" s="21"/>
-      <c r="OE1" s="21"/>
-      <c r="OF1" s="21"/>
-      <c r="OG1" s="21"/>
-      <c r="OH1" s="21"/>
-      <c r="OI1" s="21"/>
-      <c r="OJ1" s="21"/>
-      <c r="OK1" s="21"/>
-      <c r="OL1" s="21"/>
-      <c r="OM1" s="21"/>
-      <c r="ON1" s="21"/>
-      <c r="OO1" s="21"/>
-      <c r="OP1" s="21"/>
-      <c r="OQ1" s="21"/>
-      <c r="OR1" s="21"/>
-      <c r="OS1" s="21"/>
-      <c r="OT1" s="21"/>
-      <c r="OU1" s="21"/>
-      <c r="OV1" s="21"/>
-      <c r="OW1" s="21"/>
-      <c r="OX1" s="21"/>
-      <c r="OY1" s="21"/>
-      <c r="OZ1" s="21"/>
-      <c r="PA1" s="21"/>
-      <c r="PB1" s="21"/>
-      <c r="PC1" s="21"/>
-      <c r="PD1" s="21"/>
-      <c r="PE1" s="21"/>
-      <c r="PF1" s="21"/>
-      <c r="PG1" s="21"/>
-      <c r="PH1" s="21"/>
-      <c r="PI1" s="21"/>
-      <c r="PJ1" s="21"/>
-      <c r="PK1" s="21"/>
-      <c r="PL1" s="21"/>
-      <c r="PM1" s="21"/>
-      <c r="PN1" s="21"/>
-      <c r="PO1" s="21"/>
-      <c r="PP1" s="21"/>
-      <c r="PQ1" s="21"/>
-      <c r="PR1" s="21"/>
-      <c r="PS1" s="21"/>
-      <c r="PT1" s="21"/>
-      <c r="PU1" s="21"/>
-      <c r="PV1" s="21"/>
-      <c r="PW1" s="21"/>
-      <c r="PX1" s="21"/>
-      <c r="PY1" s="21"/>
-      <c r="PZ1" s="21"/>
-      <c r="QA1" s="21"/>
-      <c r="QB1" s="21"/>
-      <c r="QC1" s="21"/>
-      <c r="QD1" s="21"/>
-      <c r="QE1" s="21"/>
-      <c r="QF1" s="21"/>
-      <c r="QG1" s="21"/>
-      <c r="QH1" s="21"/>
-      <c r="QI1" s="21"/>
-      <c r="QJ1" s="21"/>
-      <c r="QK1" s="21"/>
-      <c r="QL1" s="21"/>
-      <c r="QM1" s="21"/>
-      <c r="QN1" s="21"/>
-      <c r="QO1" s="21"/>
-      <c r="QP1" s="21"/>
-      <c r="QQ1" s="21"/>
-      <c r="QR1" s="21"/>
-      <c r="QS1" s="21"/>
-      <c r="QT1" s="21"/>
-      <c r="QU1" s="21"/>
-      <c r="QV1" s="21"/>
-      <c r="QW1" s="21"/>
-      <c r="QX1" s="21"/>
-      <c r="QY1" s="21"/>
-      <c r="QZ1" s="21"/>
-      <c r="RA1" s="21"/>
-      <c r="RB1" s="21"/>
-      <c r="RC1" s="21"/>
-      <c r="RD1" s="21"/>
-      <c r="RE1" s="21"/>
-      <c r="RF1" s="21"/>
-      <c r="RG1" s="21"/>
-      <c r="RH1" s="21"/>
-      <c r="RI1" s="21"/>
-      <c r="RJ1" s="21"/>
-      <c r="RK1" s="21"/>
-      <c r="RL1" s="21"/>
-      <c r="RM1" s="21"/>
-      <c r="RN1" s="21"/>
-      <c r="RO1" s="21"/>
-      <c r="RP1" s="21"/>
-      <c r="RQ1" s="21"/>
-      <c r="RR1" s="21"/>
-      <c r="RS1" s="21"/>
-      <c r="RT1" s="21"/>
-      <c r="RU1" s="21"/>
-      <c r="RV1" s="21"/>
-      <c r="RW1" s="21"/>
-      <c r="RX1" s="21"/>
-      <c r="RY1" s="21"/>
-      <c r="RZ1" s="21"/>
-      <c r="SA1" s="21"/>
-      <c r="SB1" s="21"/>
-      <c r="SC1" s="21"/>
-      <c r="SD1" s="21"/>
-      <c r="SE1" s="21"/>
-      <c r="SF1" s="21"/>
-      <c r="SG1" s="21"/>
-      <c r="SH1" s="21"/>
-      <c r="SI1" s="21"/>
-      <c r="SJ1" s="21"/>
-      <c r="SK1" s="21"/>
-      <c r="SL1" s="21"/>
-      <c r="SM1" s="21"/>
-      <c r="SN1" s="21"/>
-      <c r="SO1" s="21"/>
-      <c r="SP1" s="21"/>
-      <c r="SQ1" s="21"/>
-      <c r="SR1" s="21"/>
-      <c r="SS1" s="21"/>
-      <c r="ST1" s="21"/>
-      <c r="SU1" s="21"/>
-      <c r="SV1" s="21"/>
-      <c r="SW1" s="21"/>
-      <c r="SX1" s="21"/>
-      <c r="SY1" s="21"/>
-      <c r="SZ1" s="21"/>
-      <c r="TA1" s="21"/>
-      <c r="TB1" s="21"/>
-      <c r="TC1" s="21"/>
-      <c r="TD1" s="21"/>
-      <c r="TE1" s="21"/>
-      <c r="TF1" s="21"/>
-      <c r="TG1" s="21"/>
-      <c r="TH1" s="21"/>
-      <c r="TI1" s="21"/>
-      <c r="TJ1" s="21"/>
-      <c r="TK1" s="21"/>
-      <c r="TL1" s="21"/>
-      <c r="TM1" s="21"/>
-      <c r="TN1" s="21"/>
-      <c r="TO1" s="21"/>
-      <c r="TP1" s="21"/>
-      <c r="TQ1" s="21"/>
-      <c r="TR1" s="21"/>
-      <c r="TS1" s="21"/>
-      <c r="TT1" s="21"/>
-      <c r="TU1" s="21"/>
-      <c r="TV1" s="21"/>
-      <c r="TW1" s="21"/>
-      <c r="TX1" s="21"/>
-      <c r="TY1" s="21"/>
-      <c r="TZ1" s="21"/>
-      <c r="UA1" s="21"/>
-      <c r="UB1" s="21"/>
-      <c r="UC1" s="21"/>
-      <c r="UD1" s="21"/>
-      <c r="UE1" s="21"/>
-      <c r="UF1" s="21"/>
-      <c r="UG1" s="21"/>
-      <c r="UH1" s="21"/>
-      <c r="UI1" s="21"/>
-      <c r="UJ1" s="21"/>
-      <c r="UK1" s="21"/>
-      <c r="UL1" s="21"/>
-      <c r="UM1" s="21"/>
-      <c r="UN1" s="21"/>
-      <c r="UO1" s="21"/>
-      <c r="UP1" s="21"/>
-      <c r="UQ1" s="21"/>
-      <c r="UR1" s="21"/>
-      <c r="US1" s="21"/>
-      <c r="UT1" s="21"/>
-      <c r="UU1" s="21"/>
-      <c r="UV1" s="21"/>
-      <c r="UW1" s="21"/>
-      <c r="UX1" s="21"/>
-      <c r="UY1" s="21"/>
-      <c r="UZ1" s="21"/>
-      <c r="VA1" s="21"/>
-      <c r="VB1" s="21"/>
-      <c r="VC1" s="21"/>
-      <c r="VD1" s="21"/>
-      <c r="VE1" s="21"/>
-      <c r="VF1" s="21"/>
-      <c r="VG1" s="21"/>
-      <c r="VH1" s="21"/>
-      <c r="VI1" s="21"/>
-      <c r="VJ1" s="21"/>
-      <c r="VK1" s="21"/>
-      <c r="VL1" s="21"/>
-      <c r="VM1" s="21"/>
-      <c r="VN1" s="21"/>
-      <c r="VO1" s="21"/>
-      <c r="VP1" s="21"/>
-      <c r="VQ1" s="21"/>
-      <c r="VR1" s="21"/>
-      <c r="VS1" s="21"/>
-      <c r="VT1" s="21"/>
-      <c r="VU1" s="21"/>
-      <c r="VV1" s="21"/>
-      <c r="VW1" s="21"/>
-      <c r="VX1" s="21"/>
-      <c r="VY1" s="21"/>
-      <c r="VZ1" s="21"/>
-      <c r="WA1" s="21"/>
-      <c r="WB1" s="21"/>
-      <c r="WC1" s="21"/>
-      <c r="WD1" s="21"/>
-      <c r="WE1" s="21"/>
-      <c r="WF1" s="21"/>
-      <c r="WG1" s="21"/>
-      <c r="WH1" s="21"/>
-      <c r="WI1" s="21"/>
-      <c r="WJ1" s="21"/>
-      <c r="WK1" s="21"/>
-      <c r="WL1" s="21"/>
-      <c r="WM1" s="21"/>
-      <c r="WN1" s="21"/>
-      <c r="WO1" s="21"/>
-      <c r="WP1" s="21"/>
-      <c r="WQ1" s="21"/>
-      <c r="WR1" s="21"/>
-      <c r="WS1" s="21"/>
-      <c r="WT1" s="21"/>
-      <c r="WU1" s="21"/>
-      <c r="WV1" s="21"/>
-      <c r="WW1" s="21"/>
-      <c r="WX1" s="21"/>
-      <c r="WY1" s="21"/>
-      <c r="WZ1" s="21"/>
-      <c r="XA1" s="21"/>
-      <c r="XB1" s="21"/>
-      <c r="XC1" s="21"/>
-      <c r="XD1" s="21"/>
-      <c r="XE1" s="21"/>
-      <c r="XF1" s="21"/>
-      <c r="XG1" s="21"/>
-      <c r="XH1" s="21"/>
-      <c r="XI1" s="21"/>
-      <c r="XJ1" s="21"/>
-      <c r="XK1" s="21"/>
-      <c r="XL1" s="21"/>
-      <c r="XM1" s="21"/>
-      <c r="XN1" s="21"/>
-      <c r="XO1" s="21"/>
-      <c r="XP1" s="21"/>
-      <c r="XQ1" s="21"/>
-      <c r="XR1" s="21"/>
-      <c r="XS1" s="21"/>
-      <c r="XT1" s="21"/>
-      <c r="XU1" s="21"/>
-      <c r="XV1" s="21"/>
-      <c r="XW1" s="21"/>
-      <c r="XX1" s="21"/>
-      <c r="XY1" s="21"/>
-      <c r="XZ1" s="21"/>
-      <c r="YA1" s="21"/>
-      <c r="YB1" s="21"/>
-      <c r="YC1" s="21"/>
-      <c r="YD1" s="21"/>
-      <c r="YE1" s="21"/>
-      <c r="YF1" s="21"/>
-      <c r="YG1" s="21"/>
-      <c r="YH1" s="21"/>
-      <c r="YI1" s="21"/>
-      <c r="YJ1" s="21"/>
-      <c r="YK1" s="21"/>
-      <c r="YL1" s="21"/>
-      <c r="YM1" s="21"/>
-      <c r="YN1" s="21"/>
-      <c r="YO1" s="21"/>
-      <c r="YP1" s="21"/>
-      <c r="YQ1" s="21"/>
-      <c r="YR1" s="21"/>
-      <c r="YS1" s="21"/>
-      <c r="YT1" s="21"/>
-      <c r="YU1" s="21"/>
-      <c r="YV1" s="21"/>
-      <c r="YW1" s="21"/>
-      <c r="YX1" s="21"/>
-      <c r="YY1" s="21"/>
-      <c r="YZ1" s="21"/>
-      <c r="ZA1" s="21"/>
-      <c r="ZB1" s="21"/>
-      <c r="ZC1" s="21"/>
-      <c r="ZD1" s="21"/>
-      <c r="ZE1" s="21"/>
-      <c r="ZF1" s="21"/>
-      <c r="ZG1" s="21"/>
-      <c r="ZH1" s="21"/>
-      <c r="ZI1" s="21"/>
-      <c r="ZJ1" s="21"/>
-      <c r="ZK1" s="21"/>
-      <c r="ZL1" s="21"/>
-      <c r="ZM1" s="21"/>
-      <c r="ZN1" s="21"/>
-      <c r="ZO1" s="21"/>
-      <c r="ZP1" s="21"/>
-      <c r="ZQ1" s="21"/>
-      <c r="ZR1" s="21"/>
-      <c r="ZS1" s="21"/>
-      <c r="ZT1" s="21"/>
-      <c r="ZU1" s="21"/>
-      <c r="ZV1" s="21"/>
-      <c r="ZW1" s="21"/>
-      <c r="ZX1" s="21"/>
-      <c r="ZY1" s="21"/>
-      <c r="ZZ1" s="21"/>
-      <c r="AAA1" s="21"/>
-      <c r="AAB1" s="21"/>
-      <c r="AAC1" s="21"/>
-      <c r="AAD1" s="21"/>
-      <c r="AAE1" s="21"/>
-      <c r="AAF1" s="21"/>
-      <c r="AAG1" s="21"/>
-      <c r="AAH1" s="21"/>
-      <c r="AAI1" s="21"/>
-      <c r="AAJ1" s="21"/>
-      <c r="AAK1" s="21"/>
-      <c r="AAL1" s="21"/>
-      <c r="AAM1" s="21"/>
-      <c r="AAN1" s="21"/>
-      <c r="AAO1" s="21"/>
-      <c r="AAP1" s="21"/>
-      <c r="AAQ1" s="21"/>
-      <c r="AAR1" s="21"/>
-      <c r="AAS1" s="21"/>
-      <c r="AAT1" s="21"/>
-      <c r="AAU1" s="21"/>
-      <c r="AAV1" s="21"/>
-      <c r="AAW1" s="21"/>
-      <c r="AAX1" s="21"/>
-      <c r="AAY1" s="21"/>
-      <c r="AAZ1" s="21"/>
-      <c r="ABA1" s="21"/>
-      <c r="ABB1" s="21"/>
-      <c r="ABC1" s="21"/>
-      <c r="ABD1" s="21"/>
-      <c r="ABE1" s="21"/>
-      <c r="ABF1" s="21"/>
-      <c r="ABG1" s="21"/>
-      <c r="ABH1" s="21"/>
-      <c r="ABI1" s="21"/>
+      <c r="FL1" s="25"/>
+      <c r="FM1" s="25"/>
+      <c r="FN1" s="25"/>
+      <c r="FO1" s="25"/>
+      <c r="FP1" s="25"/>
+      <c r="FQ1" s="25"/>
+      <c r="FR1" s="25"/>
+      <c r="FS1" s="25"/>
+      <c r="FT1" s="25"/>
+      <c r="FU1" s="25"/>
+      <c r="FV1" s="25"/>
+      <c r="FW1" s="25"/>
+      <c r="FX1" s="25"/>
+      <c r="FY1" s="25"/>
+      <c r="FZ1" s="25"/>
+      <c r="GA1" s="25"/>
+      <c r="GB1" s="25"/>
+      <c r="GC1" s="25"/>
+      <c r="GD1" s="25"/>
+      <c r="GE1" s="25"/>
+      <c r="GF1" s="25"/>
+      <c r="GG1" s="25"/>
+      <c r="GH1" s="25"/>
+      <c r="GI1" s="25"/>
+      <c r="GJ1" s="25"/>
+      <c r="GK1" s="25"/>
+      <c r="GL1" s="25"/>
+      <c r="GM1" s="25"/>
+      <c r="GN1" s="25"/>
+      <c r="GO1" s="26"/>
+      <c r="GP1" s="25"/>
+      <c r="GQ1" s="25"/>
+      <c r="GR1" s="25"/>
+      <c r="GS1" s="25"/>
+      <c r="GT1" s="25"/>
+      <c r="GU1" s="25"/>
+      <c r="GV1" s="25"/>
+      <c r="GW1" s="25"/>
+      <c r="GX1" s="25"/>
+      <c r="GY1" s="25"/>
+      <c r="GZ1" s="25"/>
+      <c r="HA1" s="25"/>
+      <c r="HB1" s="25"/>
+      <c r="HC1" s="25"/>
+      <c r="HD1" s="25"/>
+      <c r="HE1" s="25"/>
+      <c r="HF1" s="25"/>
+      <c r="HG1" s="25"/>
+      <c r="HH1" s="25"/>
+      <c r="HI1" s="25"/>
+      <c r="HJ1" s="25"/>
+      <c r="HK1" s="25"/>
+      <c r="HL1" s="25"/>
+      <c r="HM1" s="25"/>
+      <c r="HN1" s="25"/>
+      <c r="HO1" s="25"/>
+      <c r="HP1" s="25"/>
+      <c r="HQ1" s="25"/>
+      <c r="HR1" s="25"/>
+      <c r="HS1" s="25"/>
+      <c r="HT1" s="25"/>
+      <c r="HU1" s="25"/>
+      <c r="HV1" s="25"/>
+      <c r="HW1" s="25"/>
+      <c r="HX1" s="25"/>
+      <c r="HY1" s="25"/>
+      <c r="HZ1" s="25"/>
+      <c r="IA1" s="25"/>
+      <c r="IB1" s="25"/>
+      <c r="IC1" s="25"/>
+      <c r="ID1" s="25"/>
+      <c r="IE1" s="25"/>
+      <c r="IF1" s="25"/>
+      <c r="IG1" s="25"/>
+      <c r="IH1" s="25"/>
+      <c r="II1" s="25"/>
+      <c r="IJ1" s="25"/>
+      <c r="IK1" s="25"/>
+      <c r="IL1" s="25"/>
+      <c r="IM1" s="25"/>
+      <c r="IN1" s="25"/>
+      <c r="IO1" s="25"/>
+      <c r="IP1" s="25"/>
+      <c r="IQ1" s="25"/>
+      <c r="IR1" s="25"/>
+      <c r="IS1" s="25"/>
+      <c r="IT1" s="25"/>
+      <c r="IU1" s="25"/>
+      <c r="IV1" s="25"/>
+      <c r="IW1" s="25"/>
+      <c r="IX1" s="25"/>
+      <c r="IY1" s="25"/>
+      <c r="IZ1" s="25"/>
+      <c r="JA1" s="25"/>
+      <c r="JB1" s="25"/>
+      <c r="JC1" s="25"/>
+      <c r="JD1" s="25"/>
+      <c r="JE1" s="25"/>
+      <c r="JF1" s="25"/>
+      <c r="JG1" s="25"/>
+      <c r="JH1" s="25"/>
+      <c r="JI1" s="25"/>
+      <c r="JJ1" s="25"/>
+      <c r="JK1" s="25"/>
+      <c r="JL1" s="25"/>
+      <c r="JM1" s="25"/>
+      <c r="JN1" s="25"/>
+      <c r="JO1" s="25"/>
+      <c r="JP1" s="25"/>
+      <c r="JQ1" s="25"/>
+      <c r="JR1" s="25"/>
+      <c r="JS1" s="25"/>
+      <c r="JT1" s="25"/>
+      <c r="JU1" s="25"/>
+      <c r="JV1" s="25"/>
+      <c r="JW1" s="25"/>
+      <c r="JX1" s="25"/>
+      <c r="JY1" s="25"/>
+      <c r="JZ1" s="25"/>
+      <c r="KA1" s="25"/>
+      <c r="KB1" s="25"/>
+      <c r="KC1" s="25"/>
+      <c r="KD1" s="25"/>
+      <c r="KE1" s="25"/>
+      <c r="KF1" s="25"/>
+      <c r="KG1" s="25"/>
+      <c r="KH1" s="25"/>
+      <c r="KI1" s="25"/>
+      <c r="KJ1" s="25"/>
+      <c r="KK1" s="25"/>
+      <c r="KL1" s="25"/>
+      <c r="KM1" s="25"/>
+      <c r="KN1" s="25"/>
+      <c r="KO1" s="25"/>
+      <c r="KP1" s="25"/>
+      <c r="KQ1" s="25"/>
+      <c r="KR1" s="25"/>
+      <c r="KS1" s="25"/>
+      <c r="KT1" s="25"/>
+      <c r="KU1" s="25"/>
+      <c r="KV1" s="25"/>
+      <c r="KW1" s="25"/>
+      <c r="KX1" s="25"/>
+      <c r="KY1" s="25"/>
+      <c r="KZ1" s="25"/>
+      <c r="LA1" s="25"/>
+      <c r="LB1" s="25"/>
+      <c r="LC1" s="25"/>
+      <c r="LD1" s="25"/>
+      <c r="LE1" s="25"/>
+      <c r="LF1" s="25"/>
+      <c r="LG1" s="25"/>
+      <c r="LH1" s="25"/>
+      <c r="LI1" s="25"/>
+      <c r="LJ1" s="25"/>
+      <c r="LK1" s="25"/>
+      <c r="LL1" s="25"/>
+      <c r="LM1" s="25"/>
+      <c r="LN1" s="25"/>
+      <c r="LO1" s="25"/>
+      <c r="LP1" s="25"/>
+      <c r="LQ1" s="25"/>
+      <c r="LR1" s="25"/>
+      <c r="LS1" s="25"/>
+      <c r="LT1" s="25"/>
+      <c r="LU1" s="25"/>
+      <c r="LV1" s="25"/>
+      <c r="LW1" s="25"/>
+      <c r="LX1" s="25"/>
+      <c r="LY1" s="25"/>
+      <c r="LZ1" s="25"/>
+      <c r="MA1" s="25"/>
+      <c r="MB1" s="25"/>
+      <c r="MC1" s="25"/>
+      <c r="MD1" s="25"/>
+      <c r="ME1" s="25"/>
+      <c r="MF1" s="25"/>
+      <c r="MG1" s="25"/>
+      <c r="MH1" s="25"/>
+      <c r="MI1" s="25"/>
+      <c r="MJ1" s="25"/>
+      <c r="MK1" s="25"/>
+      <c r="ML1" s="25"/>
+      <c r="MM1" s="25"/>
+      <c r="MN1" s="25"/>
+      <c r="MO1" s="25"/>
+      <c r="MP1" s="25"/>
+      <c r="MQ1" s="25"/>
+      <c r="MR1" s="25"/>
+      <c r="MS1" s="25"/>
+      <c r="MT1" s="25"/>
+      <c r="MU1" s="25"/>
+      <c r="MV1" s="25"/>
+      <c r="MW1" s="25"/>
+      <c r="MX1" s="25"/>
+      <c r="MY1" s="25"/>
+      <c r="MZ1" s="25"/>
+      <c r="NA1" s="25"/>
+      <c r="NB1" s="25"/>
+      <c r="NC1" s="25"/>
+      <c r="ND1" s="25"/>
+      <c r="NE1" s="25"/>
+      <c r="NF1" s="25"/>
+      <c r="NG1" s="25"/>
+      <c r="NH1" s="25"/>
+      <c r="NI1" s="25"/>
+      <c r="NJ1" s="25"/>
+      <c r="NK1" s="25"/>
+      <c r="NL1" s="25"/>
+      <c r="NM1" s="25"/>
+      <c r="NN1" s="25"/>
+      <c r="NO1" s="25"/>
+      <c r="NP1" s="25"/>
+      <c r="NQ1" s="25"/>
+      <c r="NR1" s="25"/>
+      <c r="NS1" s="25"/>
+      <c r="NT1" s="25"/>
+      <c r="NU1" s="25"/>
+      <c r="NV1" s="25"/>
+      <c r="NW1" s="25"/>
+      <c r="NX1" s="25"/>
+      <c r="NY1" s="25"/>
+      <c r="NZ1" s="25"/>
+      <c r="OA1" s="25"/>
+      <c r="OB1" s="25"/>
+      <c r="OC1" s="25"/>
+      <c r="OD1" s="25"/>
+      <c r="OE1" s="25"/>
+      <c r="OF1" s="25"/>
+      <c r="OG1" s="25"/>
+      <c r="OH1" s="25"/>
+      <c r="OI1" s="25"/>
+      <c r="OJ1" s="25"/>
+      <c r="OK1" s="25"/>
+      <c r="OL1" s="25"/>
+      <c r="OM1" s="25"/>
+      <c r="ON1" s="25"/>
+      <c r="OO1" s="25"/>
+      <c r="OP1" s="25"/>
+      <c r="OQ1" s="25"/>
+      <c r="OR1" s="25"/>
+      <c r="OS1" s="25"/>
+      <c r="OT1" s="25"/>
+      <c r="OU1" s="25"/>
+      <c r="OV1" s="25"/>
+      <c r="OW1" s="25"/>
+      <c r="OX1" s="25"/>
+      <c r="OY1" s="25"/>
+      <c r="OZ1" s="25"/>
+      <c r="PA1" s="25"/>
+      <c r="PB1" s="25"/>
+      <c r="PC1" s="25"/>
+      <c r="PD1" s="25"/>
+      <c r="PE1" s="25"/>
+      <c r="PF1" s="25"/>
+      <c r="PG1" s="25"/>
+      <c r="PH1" s="25"/>
+      <c r="PI1" s="25"/>
+      <c r="PJ1" s="25"/>
+      <c r="PK1" s="25"/>
+      <c r="PL1" s="25"/>
+      <c r="PM1" s="25"/>
+      <c r="PN1" s="25"/>
+      <c r="PO1" s="25"/>
+      <c r="PP1" s="25"/>
+      <c r="PQ1" s="25"/>
+      <c r="PR1" s="25"/>
+      <c r="PS1" s="25"/>
+      <c r="PT1" s="25"/>
+      <c r="PU1" s="25"/>
+      <c r="PV1" s="25"/>
+      <c r="PW1" s="25"/>
+      <c r="PX1" s="25"/>
+      <c r="PY1" s="25"/>
+      <c r="PZ1" s="25"/>
+      <c r="QA1" s="25"/>
+      <c r="QB1" s="25"/>
+      <c r="QC1" s="25"/>
+      <c r="QD1" s="25"/>
+      <c r="QE1" s="25"/>
+      <c r="QF1" s="25"/>
+      <c r="QG1" s="25"/>
+      <c r="QH1" s="25"/>
+      <c r="QI1" s="25"/>
+      <c r="QJ1" s="25"/>
+      <c r="QK1" s="25"/>
+      <c r="QL1" s="25"/>
+      <c r="QM1" s="25"/>
+      <c r="QN1" s="25"/>
+      <c r="QO1" s="25"/>
+      <c r="QP1" s="25"/>
+      <c r="QQ1" s="25"/>
+      <c r="QR1" s="25"/>
+      <c r="QS1" s="25"/>
+      <c r="QT1" s="25"/>
+      <c r="QU1" s="25"/>
+      <c r="QV1" s="25"/>
+      <c r="QW1" s="25"/>
+      <c r="QX1" s="25"/>
+      <c r="QY1" s="25"/>
+      <c r="QZ1" s="25"/>
+      <c r="RA1" s="25"/>
+      <c r="RB1" s="25"/>
+      <c r="RC1" s="25"/>
+      <c r="RD1" s="25"/>
+      <c r="RE1" s="25"/>
+      <c r="RF1" s="25"/>
+      <c r="RG1" s="25"/>
+      <c r="RH1" s="25"/>
+      <c r="RI1" s="25"/>
+      <c r="RJ1" s="25"/>
+      <c r="RK1" s="25"/>
+      <c r="RL1" s="25"/>
+      <c r="RM1" s="25"/>
+      <c r="RN1" s="25"/>
+      <c r="RO1" s="25"/>
+      <c r="RP1" s="25"/>
+      <c r="RQ1" s="25"/>
+      <c r="RR1" s="25"/>
+      <c r="RS1" s="25"/>
+      <c r="RT1" s="25"/>
+      <c r="RU1" s="25"/>
+      <c r="RV1" s="25"/>
+      <c r="RW1" s="25"/>
+      <c r="RX1" s="25"/>
+      <c r="RY1" s="25"/>
+      <c r="RZ1" s="25"/>
+      <c r="SA1" s="25"/>
+      <c r="SB1" s="25"/>
+      <c r="SC1" s="25"/>
+      <c r="SD1" s="25"/>
+      <c r="SE1" s="25"/>
+      <c r="SF1" s="25"/>
+      <c r="SG1" s="25"/>
+      <c r="SH1" s="25"/>
+      <c r="SI1" s="25"/>
+      <c r="SJ1" s="25"/>
+      <c r="SK1" s="25"/>
+      <c r="SL1" s="25"/>
+      <c r="SM1" s="25"/>
+      <c r="SN1" s="25"/>
+      <c r="SO1" s="25"/>
+      <c r="SP1" s="25"/>
+      <c r="SQ1" s="25"/>
+      <c r="SR1" s="25"/>
+      <c r="SS1" s="25"/>
+      <c r="ST1" s="25"/>
+      <c r="SU1" s="25"/>
+      <c r="SV1" s="25"/>
+      <c r="SW1" s="25"/>
+      <c r="SX1" s="25"/>
+      <c r="SY1" s="25"/>
+      <c r="SZ1" s="25"/>
+      <c r="TA1" s="25"/>
+      <c r="TB1" s="25"/>
+      <c r="TC1" s="25"/>
+      <c r="TD1" s="25"/>
+      <c r="TE1" s="25"/>
+      <c r="TF1" s="25"/>
+      <c r="TG1" s="25"/>
+      <c r="TH1" s="25"/>
+      <c r="TI1" s="25"/>
+      <c r="TJ1" s="25"/>
+      <c r="TK1" s="25"/>
+      <c r="TL1" s="25"/>
+      <c r="TM1" s="25"/>
+      <c r="TN1" s="25"/>
+      <c r="TO1" s="25"/>
+      <c r="TP1" s="25"/>
+      <c r="TQ1" s="25"/>
+      <c r="TR1" s="25"/>
+      <c r="TS1" s="25"/>
+      <c r="TT1" s="25"/>
+      <c r="TU1" s="25"/>
+      <c r="TV1" s="25"/>
+      <c r="TW1" s="25"/>
+      <c r="TX1" s="25"/>
+      <c r="TY1" s="25"/>
+      <c r="TZ1" s="25"/>
+      <c r="UA1" s="25"/>
+      <c r="UB1" s="25"/>
+      <c r="UC1" s="25"/>
+      <c r="UD1" s="25"/>
+      <c r="UE1" s="25"/>
+      <c r="UF1" s="25"/>
+      <c r="UG1" s="25"/>
+      <c r="UH1" s="25"/>
+      <c r="UI1" s="25"/>
+      <c r="UJ1" s="25"/>
+      <c r="UK1" s="25"/>
+      <c r="UL1" s="25"/>
+      <c r="UM1" s="25"/>
+      <c r="UN1" s="25"/>
+      <c r="UO1" s="25"/>
+      <c r="UP1" s="25"/>
+      <c r="UQ1" s="25"/>
+      <c r="UR1" s="25"/>
+      <c r="US1" s="25"/>
+      <c r="UT1" s="25"/>
+      <c r="UU1" s="25"/>
+      <c r="UV1" s="25"/>
+      <c r="UW1" s="25"/>
+      <c r="UX1" s="25"/>
+      <c r="UY1" s="25"/>
+      <c r="UZ1" s="25"/>
+      <c r="VA1" s="25"/>
+      <c r="VB1" s="25"/>
+      <c r="VC1" s="25"/>
+      <c r="VD1" s="25"/>
+      <c r="VE1" s="25"/>
+      <c r="VF1" s="25"/>
+      <c r="VG1" s="25"/>
+      <c r="VH1" s="25"/>
+      <c r="VI1" s="25"/>
+      <c r="VJ1" s="25"/>
+      <c r="VK1" s="25"/>
+      <c r="VL1" s="25"/>
+      <c r="VM1" s="25"/>
+      <c r="VN1" s="25"/>
+      <c r="VO1" s="25"/>
+      <c r="VP1" s="25"/>
+      <c r="VQ1" s="25"/>
+      <c r="VR1" s="25"/>
+      <c r="VS1" s="25"/>
+      <c r="VT1" s="25"/>
+      <c r="VU1" s="25"/>
+      <c r="VV1" s="25"/>
+      <c r="VW1" s="25"/>
+      <c r="VX1" s="25"/>
+      <c r="VY1" s="25"/>
+      <c r="VZ1" s="25"/>
+      <c r="WA1" s="25"/>
+      <c r="WB1" s="25"/>
+      <c r="WC1" s="25"/>
+      <c r="WD1" s="25"/>
+      <c r="WE1" s="25"/>
+      <c r="WF1" s="25"/>
+      <c r="WG1" s="25"/>
+      <c r="WH1" s="25"/>
+      <c r="WI1" s="25"/>
+      <c r="WJ1" s="25"/>
+      <c r="WK1" s="25"/>
+      <c r="WL1" s="25"/>
+      <c r="WM1" s="25"/>
+      <c r="WN1" s="25"/>
+      <c r="WO1" s="25"/>
+      <c r="WP1" s="25"/>
+      <c r="WQ1" s="25"/>
+      <c r="WR1" s="25"/>
+      <c r="WS1" s="25"/>
+      <c r="WT1" s="25"/>
+      <c r="WU1" s="25"/>
+      <c r="WV1" s="25"/>
+      <c r="WW1" s="25"/>
+      <c r="WX1" s="25"/>
+      <c r="WY1" s="25"/>
+      <c r="WZ1" s="25"/>
+      <c r="XA1" s="25"/>
+      <c r="XB1" s="25"/>
+      <c r="XC1" s="25"/>
+      <c r="XD1" s="25"/>
+      <c r="XE1" s="25"/>
+      <c r="XF1" s="25"/>
+      <c r="XG1" s="25"/>
+      <c r="XH1" s="25"/>
+      <c r="XI1" s="25"/>
+      <c r="XJ1" s="25"/>
+      <c r="XK1" s="25"/>
+      <c r="XL1" s="25"/>
+      <c r="XM1" s="25"/>
+      <c r="XN1" s="25"/>
+      <c r="XO1" s="25"/>
+      <c r="XP1" s="25"/>
+      <c r="XQ1" s="25"/>
+      <c r="XR1" s="25"/>
+      <c r="XS1" s="25"/>
+      <c r="XT1" s="25"/>
+      <c r="XU1" s="25"/>
+      <c r="XV1" s="25"/>
+      <c r="XW1" s="25"/>
+      <c r="XX1" s="25"/>
+      <c r="XY1" s="25"/>
+      <c r="XZ1" s="25"/>
+      <c r="YA1" s="25"/>
+      <c r="YB1" s="25"/>
+      <c r="YC1" s="25"/>
+      <c r="YD1" s="25"/>
+      <c r="YE1" s="25"/>
+      <c r="YF1" s="25"/>
+      <c r="YG1" s="25"/>
+      <c r="YH1" s="25"/>
+      <c r="YI1" s="25"/>
+      <c r="YJ1" s="25"/>
+      <c r="YK1" s="25"/>
+      <c r="YL1" s="25"/>
+      <c r="YM1" s="25"/>
+      <c r="YN1" s="25"/>
+      <c r="YO1" s="25"/>
+      <c r="YP1" s="25"/>
+      <c r="YQ1" s="25"/>
+      <c r="YR1" s="25"/>
+      <c r="YS1" s="25"/>
+      <c r="YT1" s="25"/>
+      <c r="YU1" s="25"/>
+      <c r="YV1" s="25"/>
+      <c r="YW1" s="25"/>
+      <c r="YX1" s="25"/>
+      <c r="YY1" s="25"/>
+      <c r="YZ1" s="25"/>
+      <c r="ZA1" s="25"/>
+      <c r="ZB1" s="25"/>
+      <c r="ZC1" s="25"/>
+      <c r="ZD1" s="25"/>
+      <c r="ZE1" s="25"/>
+      <c r="ZF1" s="25"/>
+      <c r="ZG1" s="25"/>
+      <c r="ZH1" s="25"/>
+      <c r="ZI1" s="25"/>
+      <c r="ZJ1" s="25"/>
+      <c r="ZK1" s="25"/>
+      <c r="ZL1" s="25"/>
+      <c r="ZM1" s="25"/>
+      <c r="ZN1" s="25"/>
+      <c r="ZO1" s="25"/>
+      <c r="ZP1" s="25"/>
+      <c r="ZQ1" s="25"/>
+      <c r="ZR1" s="25"/>
+      <c r="ZS1" s="25"/>
+      <c r="ZT1" s="25"/>
+      <c r="ZU1" s="25"/>
+      <c r="ZV1" s="25"/>
+      <c r="ZW1" s="25"/>
+      <c r="ZX1" s="25"/>
+      <c r="ZY1" s="25"/>
+      <c r="ZZ1" s="25"/>
+      <c r="AAA1" s="25"/>
+      <c r="AAB1" s="25"/>
+      <c r="AAC1" s="25"/>
+      <c r="AAD1" s="25"/>
+      <c r="AAE1" s="25"/>
+      <c r="AAF1" s="25"/>
+      <c r="AAG1" s="25"/>
+      <c r="AAH1" s="25"/>
+      <c r="AAI1" s="25"/>
+      <c r="AAJ1" s="25"/>
+      <c r="AAK1" s="25"/>
+      <c r="AAL1" s="25"/>
+      <c r="AAM1" s="25"/>
+      <c r="AAN1" s="25"/>
+      <c r="AAO1" s="25"/>
+      <c r="AAP1" s="25"/>
+      <c r="AAQ1" s="25"/>
+      <c r="AAR1" s="25"/>
+      <c r="AAS1" s="25"/>
+      <c r="AAT1" s="25"/>
+      <c r="AAU1" s="25"/>
+      <c r="AAV1" s="25"/>
+      <c r="AAW1" s="25"/>
+      <c r="AAX1" s="25"/>
+      <c r="AAY1" s="25"/>
+      <c r="AAZ1" s="25"/>
+      <c r="ABA1" s="25"/>
+      <c r="ABB1" s="25"/>
+      <c r="ABC1" s="25"/>
+      <c r="ABD1" s="25"/>
+      <c r="ABE1" s="25"/>
+      <c r="ABF1" s="25"/>
+      <c r="ABG1" s="25"/>
+      <c r="ABH1" s="25"/>
+      <c r="ABI1" s="25"/>
     </row>
     <row r="2" spans="1:737" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -6980,12 +7054,25 @@
       <c r="GN26" s="10"/>
       <c r="GO26" s="12"/>
     </row>
-    <row r="31" spans="1:197" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:197" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="E29" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:197" ht="21" x14ac:dyDescent="0.4">
+      <c r="E30" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:197" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A31" t="s">
         <v>42</v>
       </c>
+      <c r="E31" s="23" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -6993,7 +7080,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -7001,7 +7088,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:74" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -7009,33 +7096,2340 @@
         <v>41</v>
       </c>
     </row>
+    <row r="39" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
+      <c r="T39" s="25"/>
+      <c r="U39" s="25"/>
+      <c r="V39" s="25"/>
+      <c r="W39" s="25"/>
+      <c r="X39" s="25"/>
+      <c r="Y39" s="25"/>
+      <c r="Z39" s="25"/>
+      <c r="AA39" s="25"/>
+      <c r="AB39" s="25"/>
+      <c r="AC39" s="25"/>
+      <c r="AD39" s="25"/>
+      <c r="AE39" s="25"/>
+      <c r="AF39" s="25"/>
+      <c r="AG39" s="25"/>
+      <c r="AH39" s="25"/>
+      <c r="AI39" s="25"/>
+      <c r="AJ39" s="25"/>
+      <c r="AK39" s="25"/>
+      <c r="AL39" s="25"/>
+      <c r="AM39" s="25"/>
+      <c r="AN39" s="25"/>
+      <c r="AO39" s="25"/>
+      <c r="AP39" s="25"/>
+      <c r="AQ39" s="25"/>
+      <c r="AR39" s="26"/>
+      <c r="AS39" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT39" s="25"/>
+      <c r="AU39" s="25"/>
+      <c r="AV39" s="25"/>
+      <c r="AW39" s="25"/>
+      <c r="AX39" s="25"/>
+      <c r="AY39" s="25"/>
+      <c r="AZ39" s="25"/>
+      <c r="BA39" s="25"/>
+      <c r="BB39" s="25"/>
+      <c r="BC39" s="25"/>
+      <c r="BD39" s="25"/>
+      <c r="BE39" s="25"/>
+      <c r="BF39" s="25"/>
+      <c r="BG39" s="25"/>
+      <c r="BH39" s="25"/>
+      <c r="BI39" s="25"/>
+      <c r="BJ39" s="25"/>
+      <c r="BK39" s="25"/>
+      <c r="BL39" s="25"/>
+      <c r="BM39" s="25"/>
+      <c r="BN39" s="25"/>
+      <c r="BO39" s="25"/>
+      <c r="BP39" s="25"/>
+      <c r="BQ39" s="25"/>
+      <c r="BR39" s="25"/>
+      <c r="BS39" s="25"/>
+      <c r="BT39" s="25"/>
+      <c r="BU39" s="25"/>
+      <c r="BV39" s="26"/>
+    </row>
+    <row r="40" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G40" s="2">
+        <v>24</v>
+      </c>
+      <c r="H40" s="2">
+        <v>25</v>
+      </c>
+      <c r="I40" s="2">
+        <v>26</v>
+      </c>
+      <c r="J40" s="2">
+        <v>27</v>
+      </c>
+      <c r="K40" s="2">
+        <v>28</v>
+      </c>
+      <c r="L40" s="2">
+        <v>29</v>
+      </c>
+      <c r="M40" s="3">
+        <v>30</v>
+      </c>
+      <c r="N40" s="2">
+        <v>1</v>
+      </c>
+      <c r="O40" s="2">
+        <v>2</v>
+      </c>
+      <c r="P40" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>4</v>
+      </c>
+      <c r="R40" s="2">
+        <v>5</v>
+      </c>
+      <c r="S40" s="2">
+        <v>6</v>
+      </c>
+      <c r="T40" s="2">
+        <v>7</v>
+      </c>
+      <c r="U40" s="2">
+        <v>8</v>
+      </c>
+      <c r="V40" s="2">
+        <v>9</v>
+      </c>
+      <c r="W40" s="2">
+        <v>10</v>
+      </c>
+      <c r="X40" s="2">
+        <v>11</v>
+      </c>
+      <c r="Y40" s="2">
+        <v>12</v>
+      </c>
+      <c r="Z40" s="2">
+        <v>13</v>
+      </c>
+      <c r="AA40" s="2">
+        <v>14</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>15</v>
+      </c>
+      <c r="AC40" s="2">
+        <v>16</v>
+      </c>
+      <c r="AD40" s="2">
+        <v>17</v>
+      </c>
+      <c r="AE40" s="2">
+        <v>18</v>
+      </c>
+      <c r="AF40" s="2">
+        <v>19</v>
+      </c>
+      <c r="AG40" s="2">
+        <v>20</v>
+      </c>
+      <c r="AH40" s="2">
+        <v>21</v>
+      </c>
+      <c r="AI40" s="2">
+        <v>22</v>
+      </c>
+      <c r="AJ40" s="2">
+        <v>23</v>
+      </c>
+      <c r="AK40" s="2">
+        <v>24</v>
+      </c>
+      <c r="AL40" s="2">
+        <v>25</v>
+      </c>
+      <c r="AM40" s="2">
+        <v>26</v>
+      </c>
+      <c r="AN40" s="2">
+        <v>27</v>
+      </c>
+      <c r="AO40" s="2">
+        <v>28</v>
+      </c>
+      <c r="AP40" s="2">
+        <v>29</v>
+      </c>
+      <c r="AQ40" s="2">
+        <v>30</v>
+      </c>
+      <c r="AR40" s="3">
+        <v>31</v>
+      </c>
+      <c r="AS40" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT40" s="2">
+        <v>2</v>
+      </c>
+      <c r="AU40" s="2">
+        <v>3</v>
+      </c>
+      <c r="AV40" s="2">
+        <v>4</v>
+      </c>
+      <c r="AW40" s="2">
+        <v>5</v>
+      </c>
+      <c r="AX40" s="2">
+        <v>6</v>
+      </c>
+      <c r="AY40" s="2">
+        <v>7</v>
+      </c>
+      <c r="AZ40" s="2">
+        <v>8</v>
+      </c>
+      <c r="BA40" s="2">
+        <v>9</v>
+      </c>
+      <c r="BB40" s="2">
+        <v>10</v>
+      </c>
+      <c r="BC40" s="2">
+        <v>11</v>
+      </c>
+      <c r="BD40" s="2">
+        <v>12</v>
+      </c>
+      <c r="BE40" s="2">
+        <v>13</v>
+      </c>
+      <c r="BF40" s="2">
+        <v>14</v>
+      </c>
+      <c r="BG40" s="2">
+        <v>15</v>
+      </c>
+      <c r="BH40" s="2">
+        <v>16</v>
+      </c>
+      <c r="BI40" s="2">
+        <v>17</v>
+      </c>
+      <c r="BJ40" s="2">
+        <v>18</v>
+      </c>
+      <c r="BK40" s="2">
+        <v>19</v>
+      </c>
+      <c r="BL40" s="2">
+        <v>20</v>
+      </c>
+      <c r="BM40" s="2">
+        <v>21</v>
+      </c>
+      <c r="BN40" s="2">
+        <v>22</v>
+      </c>
+      <c r="BO40" s="2">
+        <v>23</v>
+      </c>
+      <c r="BP40" s="2">
+        <v>24</v>
+      </c>
+      <c r="BQ40" s="2">
+        <v>25</v>
+      </c>
+      <c r="BR40" s="2">
+        <v>26</v>
+      </c>
+      <c r="BS40" s="2">
+        <v>27</v>
+      </c>
+      <c r="BT40" s="2">
+        <v>28</v>
+      </c>
+      <c r="BU40" s="2">
+        <v>29</v>
+      </c>
+      <c r="BV40" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="5"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="4"/>
+      <c r="Z41" s="4"/>
+      <c r="AA41" s="4"/>
+      <c r="AB41" s="4"/>
+      <c r="AC41" s="4"/>
+      <c r="AD41" s="5"/>
+      <c r="AE41" s="5"/>
+      <c r="AF41" s="4"/>
+      <c r="AG41" s="4"/>
+      <c r="AH41" s="4"/>
+      <c r="AI41" s="4"/>
+      <c r="AJ41" s="4"/>
+      <c r="AK41" s="5"/>
+      <c r="AL41" s="5"/>
+      <c r="AM41" s="4"/>
+      <c r="AN41" s="4"/>
+      <c r="AO41" s="4"/>
+      <c r="AP41" s="4"/>
+      <c r="AQ41" s="4"/>
+      <c r="AR41" s="7"/>
+      <c r="AS41" s="5"/>
+      <c r="AT41" s="4"/>
+      <c r="AU41" s="4"/>
+      <c r="AV41" s="4"/>
+      <c r="AW41" s="4"/>
+      <c r="AX41" s="4"/>
+      <c r="AY41" s="5"/>
+      <c r="AZ41" s="5"/>
+      <c r="BA41" s="4"/>
+      <c r="BB41" s="4"/>
+      <c r="BC41" s="4"/>
+      <c r="BD41" s="4"/>
+      <c r="BE41" s="4"/>
+      <c r="BF41" s="5"/>
+      <c r="BG41" s="5"/>
+      <c r="BH41" s="4"/>
+      <c r="BI41" s="4"/>
+      <c r="BJ41" s="4"/>
+      <c r="BK41" s="4"/>
+      <c r="BL41" s="4"/>
+      <c r="BM41" s="5"/>
+      <c r="BN41" s="5"/>
+      <c r="BO41" s="4"/>
+      <c r="BP41" s="4"/>
+      <c r="BQ41" s="4"/>
+      <c r="BR41" s="4"/>
+      <c r="BS41" s="4"/>
+      <c r="BT41" s="5"/>
+      <c r="BU41" s="5"/>
+      <c r="BV41" s="6"/>
+    </row>
+    <row r="42" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="4">
+        <v>3</v>
+      </c>
+      <c r="E42" s="14">
+        <v>45772</v>
+      </c>
+      <c r="F42" s="14">
+        <v>45774</v>
+      </c>
+      <c r="G42" s="27"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="5"/>
+      <c r="X42" s="5"/>
+      <c r="Y42" s="4"/>
+      <c r="Z42" s="4"/>
+      <c r="AA42" s="4"/>
+      <c r="AB42" s="4"/>
+      <c r="AC42" s="4"/>
+      <c r="AD42" s="5"/>
+      <c r="AE42" s="5"/>
+      <c r="AF42" s="4"/>
+      <c r="AG42" s="4"/>
+      <c r="AH42" s="4"/>
+      <c r="AI42" s="4"/>
+      <c r="AJ42" s="4"/>
+      <c r="AK42" s="5"/>
+      <c r="AL42" s="5"/>
+      <c r="AM42" s="4"/>
+      <c r="AN42" s="4"/>
+      <c r="AO42" s="4"/>
+      <c r="AP42" s="4"/>
+      <c r="AQ42" s="4"/>
+      <c r="AR42" s="7"/>
+      <c r="AS42" s="5"/>
+      <c r="AT42" s="4"/>
+      <c r="AU42" s="4"/>
+      <c r="AV42" s="4"/>
+      <c r="AW42" s="4"/>
+      <c r="AX42" s="4"/>
+      <c r="AY42" s="5"/>
+      <c r="AZ42" s="5"/>
+      <c r="BA42" s="4"/>
+      <c r="BB42" s="4"/>
+      <c r="BC42" s="4"/>
+      <c r="BD42" s="4"/>
+      <c r="BE42" s="4"/>
+      <c r="BF42" s="5"/>
+      <c r="BG42" s="5"/>
+      <c r="BH42" s="4"/>
+      <c r="BI42" s="4"/>
+      <c r="BJ42" s="4"/>
+      <c r="BK42" s="4"/>
+      <c r="BL42" s="4"/>
+      <c r="BM42" s="5"/>
+      <c r="BN42" s="5"/>
+      <c r="BO42" s="4"/>
+      <c r="BP42" s="4"/>
+      <c r="BQ42" s="4"/>
+      <c r="BR42" s="4"/>
+      <c r="BS42" s="4"/>
+      <c r="BT42" s="5"/>
+      <c r="BU42" s="5"/>
+      <c r="BV42" s="6"/>
+    </row>
+    <row r="43" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="5"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="4"/>
+      <c r="Z43" s="4"/>
+      <c r="AA43" s="4"/>
+      <c r="AB43" s="4"/>
+      <c r="AC43" s="4"/>
+      <c r="AD43" s="5"/>
+      <c r="AE43" s="5"/>
+      <c r="AF43" s="4"/>
+      <c r="AG43" s="4"/>
+      <c r="AH43" s="4"/>
+      <c r="AI43" s="4"/>
+      <c r="AJ43" s="4"/>
+      <c r="AK43" s="5"/>
+      <c r="AL43" s="5"/>
+      <c r="AM43" s="4"/>
+      <c r="AN43" s="4"/>
+      <c r="AO43" s="4"/>
+      <c r="AP43" s="4"/>
+      <c r="AQ43" s="4"/>
+      <c r="AR43" s="7"/>
+      <c r="AS43" s="5"/>
+      <c r="AT43" s="4"/>
+      <c r="AU43" s="4"/>
+      <c r="AV43" s="4"/>
+      <c r="AW43" s="4"/>
+      <c r="AX43" s="4"/>
+      <c r="AY43" s="5"/>
+      <c r="AZ43" s="5"/>
+      <c r="BA43" s="4"/>
+      <c r="BB43" s="4"/>
+      <c r="BC43" s="4"/>
+      <c r="BD43" s="4"/>
+      <c r="BE43" s="4"/>
+      <c r="BF43" s="5"/>
+      <c r="BG43" s="5"/>
+      <c r="BH43" s="4"/>
+      <c r="BI43" s="4"/>
+      <c r="BJ43" s="4"/>
+      <c r="BK43" s="4"/>
+      <c r="BL43" s="4"/>
+      <c r="BM43" s="5"/>
+      <c r="BN43" s="5"/>
+      <c r="BO43" s="4"/>
+      <c r="BP43" s="4"/>
+      <c r="BQ43" s="4"/>
+      <c r="BR43" s="4"/>
+      <c r="BS43" s="4"/>
+      <c r="BT43" s="5"/>
+      <c r="BU43" s="5"/>
+      <c r="BV43" s="6"/>
+    </row>
+    <row r="44" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="4">
+        <v>35</v>
+      </c>
+      <c r="E44" s="14">
+        <v>45773</v>
+      </c>
+      <c r="F44" s="14">
+        <v>45807</v>
+      </c>
+      <c r="G44" s="4"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="27"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="4"/>
+      <c r="Z44" s="4"/>
+      <c r="AA44" s="4"/>
+      <c r="AB44" s="4"/>
+      <c r="AC44" s="4"/>
+      <c r="AD44" s="5"/>
+      <c r="AE44" s="5"/>
+      <c r="AF44" s="4"/>
+      <c r="AG44" s="4"/>
+      <c r="AH44" s="4"/>
+      <c r="AI44" s="4"/>
+      <c r="AJ44" s="4"/>
+      <c r="AK44" s="5"/>
+      <c r="AL44" s="5"/>
+      <c r="AM44" s="4"/>
+      <c r="AN44" s="4"/>
+      <c r="AO44" s="4"/>
+      <c r="AP44" s="4"/>
+      <c r="AQ44" s="4"/>
+      <c r="AR44" s="7"/>
+      <c r="AS44" s="5"/>
+      <c r="AT44" s="4"/>
+      <c r="AU44" s="4"/>
+      <c r="AV44" s="4"/>
+      <c r="AW44" s="4"/>
+      <c r="AX44" s="4"/>
+      <c r="AY44" s="5"/>
+      <c r="AZ44" s="5"/>
+      <c r="BA44" s="4"/>
+      <c r="BB44" s="4"/>
+      <c r="BC44" s="4"/>
+      <c r="BD44" s="4"/>
+      <c r="BE44" s="4"/>
+      <c r="BF44" s="5"/>
+      <c r="BG44" s="5"/>
+      <c r="BH44" s="4"/>
+      <c r="BI44" s="4"/>
+      <c r="BJ44" s="4"/>
+      <c r="BK44" s="4"/>
+      <c r="BL44" s="4"/>
+      <c r="BM44" s="5"/>
+      <c r="BN44" s="5"/>
+      <c r="BO44" s="4"/>
+      <c r="BP44" s="4"/>
+      <c r="BQ44" s="4"/>
+      <c r="BR44" s="4"/>
+      <c r="BS44" s="4"/>
+      <c r="BT44" s="5"/>
+      <c r="BU44" s="5"/>
+      <c r="BV44" s="6"/>
+    </row>
+    <row r="45" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="4"/>
+      <c r="Z45" s="4"/>
+      <c r="AA45" s="4"/>
+      <c r="AB45" s="4"/>
+      <c r="AC45" s="4"/>
+      <c r="AD45" s="5"/>
+      <c r="AE45" s="5"/>
+      <c r="AF45" s="4"/>
+      <c r="AG45" s="4"/>
+      <c r="AH45" s="4"/>
+      <c r="AI45" s="4"/>
+      <c r="AJ45" s="4"/>
+      <c r="AK45" s="5"/>
+      <c r="AL45" s="5"/>
+      <c r="AM45" s="4"/>
+      <c r="AN45" s="4"/>
+      <c r="AO45" s="4"/>
+      <c r="AP45" s="4"/>
+      <c r="AQ45" s="4"/>
+      <c r="AR45" s="7"/>
+      <c r="AS45" s="5"/>
+      <c r="AT45" s="4"/>
+      <c r="AU45" s="4"/>
+      <c r="AV45" s="4"/>
+      <c r="AW45" s="4"/>
+      <c r="AX45" s="4"/>
+      <c r="AY45" s="5"/>
+      <c r="AZ45" s="5"/>
+      <c r="BA45" s="4"/>
+      <c r="BB45" s="4"/>
+      <c r="BC45" s="4"/>
+      <c r="BD45" s="4"/>
+      <c r="BE45" s="4"/>
+      <c r="BF45" s="5"/>
+      <c r="BG45" s="5"/>
+      <c r="BH45" s="4"/>
+      <c r="BI45" s="4"/>
+      <c r="BJ45" s="4"/>
+      <c r="BK45" s="4"/>
+      <c r="BL45" s="4"/>
+      <c r="BM45" s="5"/>
+      <c r="BN45" s="5"/>
+      <c r="BO45" s="4"/>
+      <c r="BP45" s="4"/>
+      <c r="BQ45" s="4"/>
+      <c r="BR45" s="4"/>
+      <c r="BS45" s="4"/>
+      <c r="BT45" s="5"/>
+      <c r="BU45" s="5"/>
+      <c r="BV45" s="6"/>
+    </row>
+    <row r="46" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="4">
+        <v>7</v>
+      </c>
+      <c r="E46" s="14">
+        <v>45781</v>
+      </c>
+      <c r="F46" s="14">
+        <v>45787</v>
+      </c>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="8"/>
+      <c r="S46" s="8"/>
+      <c r="T46" s="8"/>
+      <c r="U46" s="8"/>
+      <c r="V46" s="8"/>
+      <c r="W46" s="8"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="27"/>
+      <c r="Z46" s="4"/>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="4"/>
+      <c r="AD46" s="5"/>
+      <c r="AE46" s="5"/>
+      <c r="AF46" s="4"/>
+      <c r="AG46" s="4"/>
+      <c r="AH46" s="4"/>
+      <c r="AI46" s="4"/>
+      <c r="AJ46" s="4"/>
+      <c r="AK46" s="5"/>
+      <c r="AL46" s="5"/>
+      <c r="AM46" s="4"/>
+      <c r="AN46" s="4"/>
+      <c r="AO46" s="4"/>
+      <c r="AP46" s="4"/>
+      <c r="AQ46" s="4"/>
+      <c r="AR46" s="7"/>
+      <c r="AS46" s="5"/>
+      <c r="AT46" s="4"/>
+      <c r="AU46" s="4"/>
+      <c r="AV46" s="4"/>
+      <c r="AW46" s="4"/>
+      <c r="AX46" s="4"/>
+      <c r="AY46" s="5"/>
+      <c r="AZ46" s="5"/>
+      <c r="BA46" s="4"/>
+      <c r="BB46" s="4"/>
+      <c r="BC46" s="4"/>
+      <c r="BD46" s="4"/>
+      <c r="BE46" s="4"/>
+      <c r="BF46" s="5"/>
+      <c r="BG46" s="5"/>
+      <c r="BH46" s="4"/>
+      <c r="BI46" s="4"/>
+      <c r="BJ46" s="4"/>
+      <c r="BK46" s="4"/>
+      <c r="BL46" s="4"/>
+      <c r="BM46" s="5"/>
+      <c r="BN46" s="5"/>
+      <c r="BO46" s="4"/>
+      <c r="BP46" s="4"/>
+      <c r="BQ46" s="4"/>
+      <c r="BR46" s="4"/>
+      <c r="BS46" s="4"/>
+      <c r="BT46" s="5"/>
+      <c r="BU46" s="5"/>
+      <c r="BV46" s="6"/>
+    </row>
+    <row r="47" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="4">
+        <v>18</v>
+      </c>
+      <c r="E47" s="14">
+        <v>45791</v>
+      </c>
+      <c r="F47" s="14">
+        <v>45808</v>
+      </c>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="27"/>
+      <c r="AA47" s="8"/>
+      <c r="AB47" s="8"/>
+      <c r="AC47" s="8"/>
+      <c r="AD47" s="8"/>
+      <c r="AE47" s="8"/>
+      <c r="AF47" s="8"/>
+      <c r="AG47" s="8"/>
+      <c r="AH47" s="8"/>
+      <c r="AI47" s="8"/>
+      <c r="AJ47" s="8"/>
+      <c r="AK47" s="8"/>
+      <c r="AL47" s="8"/>
+      <c r="AM47" s="8"/>
+      <c r="AN47" s="8"/>
+      <c r="AO47" s="8"/>
+      <c r="AP47" s="8"/>
+      <c r="AQ47" s="8"/>
+      <c r="AR47" s="8"/>
+      <c r="AS47" s="5"/>
+      <c r="AT47" s="4"/>
+      <c r="AU47" s="4"/>
+      <c r="AV47" s="4"/>
+      <c r="AW47" s="4"/>
+      <c r="AX47" s="4"/>
+      <c r="AY47" s="5"/>
+      <c r="AZ47" s="5"/>
+      <c r="BA47" s="4"/>
+      <c r="BB47" s="4"/>
+      <c r="BC47" s="4"/>
+      <c r="BD47" s="4"/>
+      <c r="BE47" s="4"/>
+      <c r="BF47" s="5"/>
+      <c r="BG47" s="5"/>
+      <c r="BH47" s="4"/>
+      <c r="BI47" s="4"/>
+      <c r="BJ47" s="4"/>
+      <c r="BK47" s="4"/>
+      <c r="BL47" s="4"/>
+      <c r="BM47" s="5"/>
+      <c r="BN47" s="5"/>
+      <c r="BO47" s="4"/>
+      <c r="BP47" s="4"/>
+      <c r="BQ47" s="4"/>
+      <c r="BR47" s="4"/>
+      <c r="BS47" s="4"/>
+      <c r="BT47" s="5"/>
+      <c r="BU47" s="5"/>
+      <c r="BV47" s="6"/>
+    </row>
+    <row r="48" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="4"/>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="4"/>
+      <c r="Z48" s="4"/>
+      <c r="AA48" s="4"/>
+      <c r="AB48" s="4"/>
+      <c r="AC48" s="4"/>
+      <c r="AD48" s="5"/>
+      <c r="AE48" s="5"/>
+      <c r="AF48" s="4"/>
+      <c r="AG48" s="4"/>
+      <c r="AH48" s="4"/>
+      <c r="AI48" s="4"/>
+      <c r="AJ48" s="4"/>
+      <c r="AK48" s="5"/>
+      <c r="AL48" s="5"/>
+      <c r="AM48" s="4"/>
+      <c r="AN48" s="4"/>
+      <c r="AO48" s="4"/>
+      <c r="AP48" s="4"/>
+      <c r="AQ48" s="4"/>
+      <c r="AR48" s="7"/>
+      <c r="AS48" s="5"/>
+      <c r="AT48" s="4"/>
+      <c r="AU48" s="4"/>
+      <c r="AV48" s="4"/>
+      <c r="AW48" s="4"/>
+      <c r="AX48" s="4"/>
+      <c r="AY48" s="5"/>
+      <c r="AZ48" s="5"/>
+      <c r="BA48" s="4"/>
+      <c r="BB48" s="4"/>
+      <c r="BC48" s="4"/>
+      <c r="BD48" s="4"/>
+      <c r="BE48" s="4"/>
+      <c r="BF48" s="5"/>
+      <c r="BG48" s="5"/>
+      <c r="BH48" s="4"/>
+      <c r="BI48" s="4"/>
+      <c r="BJ48" s="4"/>
+      <c r="BK48" s="4"/>
+      <c r="BL48" s="4"/>
+      <c r="BM48" s="5"/>
+      <c r="BN48" s="5"/>
+      <c r="BO48" s="4"/>
+      <c r="BP48" s="4"/>
+      <c r="BQ48" s="4"/>
+      <c r="BR48" s="4"/>
+      <c r="BS48" s="4"/>
+      <c r="BT48" s="5"/>
+      <c r="BU48" s="5"/>
+      <c r="BV48" s="6"/>
+    </row>
+    <row r="49" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="4">
+        <v>2</v>
+      </c>
+      <c r="E49" s="14">
+        <v>45816</v>
+      </c>
+      <c r="F49" s="14">
+        <v>45817</v>
+      </c>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AB49" s="4"/>
+      <c r="AC49" s="4"/>
+      <c r="AD49" s="4"/>
+      <c r="AE49" s="4"/>
+      <c r="AF49" s="4"/>
+      <c r="AG49" s="4"/>
+      <c r="AH49" s="4"/>
+      <c r="AI49" s="4"/>
+      <c r="AJ49" s="4"/>
+      <c r="AK49" s="5"/>
+      <c r="AL49" s="5"/>
+      <c r="AM49" s="4"/>
+      <c r="AN49" s="4"/>
+      <c r="AO49" s="4"/>
+      <c r="AP49" s="4"/>
+      <c r="AQ49" s="4"/>
+      <c r="AR49" s="7"/>
+      <c r="AS49" s="5"/>
+      <c r="AT49" s="27"/>
+      <c r="AU49" s="4"/>
+      <c r="AV49" s="4"/>
+      <c r="AW49" s="4"/>
+      <c r="AX49" s="4"/>
+      <c r="AY49" s="5"/>
+      <c r="AZ49" s="18"/>
+      <c r="BA49" s="18"/>
+      <c r="BB49" s="4"/>
+      <c r="BC49" s="4"/>
+      <c r="BD49" s="4"/>
+      <c r="BE49" s="4"/>
+      <c r="BF49" s="5"/>
+      <c r="BG49" s="5"/>
+      <c r="BH49" s="4"/>
+      <c r="BI49" s="4"/>
+      <c r="BJ49" s="4"/>
+      <c r="BK49" s="4"/>
+      <c r="BL49" s="4"/>
+      <c r="BM49" s="5"/>
+      <c r="BN49" s="5"/>
+      <c r="BO49" s="4"/>
+      <c r="BP49" s="4"/>
+      <c r="BQ49" s="4"/>
+      <c r="BR49" s="4"/>
+      <c r="BS49" s="4"/>
+      <c r="BT49" s="5"/>
+      <c r="BU49" s="5"/>
+      <c r="BV49" s="6"/>
+    </row>
+    <row r="50" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="4">
+        <v>5</v>
+      </c>
+      <c r="E50" s="14">
+        <v>45818</v>
+      </c>
+      <c r="F50" s="14">
+        <v>45822</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="5"/>
+      <c r="X50" s="5"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+      <c r="AB50" s="4"/>
+      <c r="AC50" s="4"/>
+      <c r="AD50" s="5"/>
+      <c r="AE50" s="5"/>
+      <c r="AF50" s="4"/>
+      <c r="AG50" s="4"/>
+      <c r="AH50" s="4"/>
+      <c r="AI50" s="4"/>
+      <c r="AJ50" s="4"/>
+      <c r="AK50" s="4"/>
+      <c r="AL50" s="4"/>
+      <c r="AM50" s="4"/>
+      <c r="AN50" s="4"/>
+      <c r="AO50" s="4"/>
+      <c r="AP50" s="4"/>
+      <c r="AQ50" s="4"/>
+      <c r="AR50" s="4"/>
+      <c r="AS50" s="5"/>
+      <c r="AT50" s="4"/>
+      <c r="AU50" s="4"/>
+      <c r="AV50" s="4"/>
+      <c r="AW50" s="4"/>
+      <c r="AX50" s="5"/>
+      <c r="AY50" s="5"/>
+      <c r="AZ50" s="27"/>
+      <c r="BB50" s="18"/>
+      <c r="BC50" s="18"/>
+      <c r="BD50" s="18"/>
+      <c r="BE50" s="18"/>
+      <c r="BF50" s="18"/>
+      <c r="BG50" s="4"/>
+      <c r="BH50" s="4"/>
+      <c r="BI50" s="4"/>
+      <c r="BJ50" s="4"/>
+      <c r="BK50" s="4"/>
+      <c r="BL50" s="5"/>
+      <c r="BM50" s="5"/>
+      <c r="BN50" s="4"/>
+      <c r="BO50" s="4"/>
+      <c r="BP50" s="4"/>
+      <c r="BQ50" s="4"/>
+      <c r="BR50" s="4"/>
+      <c r="BS50" s="5"/>
+      <c r="BT50" s="5"/>
+      <c r="BU50" s="6"/>
+      <c r="BV50" s="4"/>
+    </row>
+    <row r="51" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="4">
+        <v>5</v>
+      </c>
+      <c r="E51" s="14">
+        <v>45821</v>
+      </c>
+      <c r="F51" s="14">
+        <v>45825</v>
+      </c>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+      <c r="W51" s="5"/>
+      <c r="X51" s="5"/>
+      <c r="Y51" s="4"/>
+      <c r="Z51" s="4"/>
+      <c r="AA51" s="4"/>
+      <c r="AB51" s="4"/>
+      <c r="AC51" s="4"/>
+      <c r="AD51" s="5"/>
+      <c r="AE51" s="5"/>
+      <c r="AF51" s="4"/>
+      <c r="AG51" s="4"/>
+      <c r="AH51" s="4"/>
+      <c r="AI51" s="4"/>
+      <c r="AJ51" s="4"/>
+      <c r="AK51" s="5"/>
+      <c r="AL51" s="5"/>
+      <c r="AM51" s="4"/>
+      <c r="AN51" s="4"/>
+      <c r="AO51" s="4"/>
+      <c r="AP51" s="4"/>
+      <c r="AQ51" s="4"/>
+      <c r="AR51" s="7"/>
+      <c r="AS51" s="5"/>
+      <c r="AT51" s="4"/>
+      <c r="AU51" s="4"/>
+      <c r="AV51" s="4"/>
+      <c r="AW51" s="4"/>
+      <c r="AX51" s="4"/>
+      <c r="AY51" s="5"/>
+      <c r="AZ51" s="5"/>
+      <c r="BA51" s="4"/>
+      <c r="BB51" s="4"/>
+      <c r="BC51" s="4"/>
+      <c r="BD51" s="4"/>
+      <c r="BE51" s="18"/>
+      <c r="BF51" s="18"/>
+      <c r="BG51" s="18"/>
+      <c r="BH51" s="18"/>
+      <c r="BI51" s="18"/>
+      <c r="BJ51" s="4"/>
+      <c r="BK51" s="4"/>
+      <c r="BL51" s="4"/>
+      <c r="BM51" s="5"/>
+      <c r="BN51" s="5"/>
+      <c r="BO51" s="4"/>
+      <c r="BP51" s="4"/>
+      <c r="BQ51" s="4"/>
+      <c r="BR51" s="4"/>
+      <c r="BS51" s="4"/>
+      <c r="BT51" s="5"/>
+      <c r="BU51" s="5"/>
+      <c r="BV51" s="6"/>
+    </row>
+    <row r="52" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D52" s="4">
+        <v>7</v>
+      </c>
+      <c r="E52" s="14">
+        <v>45822</v>
+      </c>
+      <c r="F52" s="14">
+        <v>45828</v>
+      </c>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="4"/>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="5"/>
+      <c r="X52" s="5"/>
+      <c r="Y52" s="4"/>
+      <c r="Z52" s="4"/>
+      <c r="AA52" s="4"/>
+      <c r="AB52" s="4"/>
+      <c r="AC52" s="4"/>
+      <c r="AD52" s="5"/>
+      <c r="AE52" s="5"/>
+      <c r="AF52" s="4"/>
+      <c r="AG52" s="4"/>
+      <c r="AH52" s="4"/>
+      <c r="AI52" s="4"/>
+      <c r="AJ52" s="4"/>
+      <c r="AK52" s="5"/>
+      <c r="AL52" s="5"/>
+      <c r="AM52" s="4"/>
+      <c r="AN52" s="4"/>
+      <c r="AO52" s="4"/>
+      <c r="AP52" s="4"/>
+      <c r="AQ52" s="4"/>
+      <c r="AR52" s="7"/>
+      <c r="AS52" s="5"/>
+      <c r="AT52" s="4"/>
+      <c r="AU52" s="4"/>
+      <c r="AV52" s="4"/>
+      <c r="AW52" s="4"/>
+      <c r="AX52" s="4"/>
+      <c r="AY52" s="5"/>
+      <c r="AZ52" s="5"/>
+      <c r="BA52" s="4"/>
+      <c r="BB52" s="4"/>
+      <c r="BC52" s="4"/>
+      <c r="BD52" s="4"/>
+      <c r="BE52" s="27"/>
+      <c r="BF52" s="18"/>
+      <c r="BG52" s="18"/>
+      <c r="BH52" s="18"/>
+      <c r="BI52" s="18"/>
+      <c r="BJ52" s="18"/>
+      <c r="BK52" s="18"/>
+      <c r="BL52" s="18"/>
+      <c r="BM52" s="5"/>
+      <c r="BN52" s="5"/>
+      <c r="BO52" s="4"/>
+      <c r="BP52" s="4"/>
+      <c r="BQ52" s="4"/>
+      <c r="BR52" s="4"/>
+      <c r="BS52" s="4"/>
+      <c r="BT52" s="5"/>
+      <c r="BU52" s="5"/>
+      <c r="BV52" s="6"/>
+    </row>
+    <row r="53" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="4">
+        <v>4</v>
+      </c>
+      <c r="E53" s="14">
+        <v>45826</v>
+      </c>
+      <c r="F53" s="14">
+        <v>45829</v>
+      </c>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="4"/>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4"/>
+      <c r="W53" s="5"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="4"/>
+      <c r="Z53" s="4"/>
+      <c r="AA53" s="4"/>
+      <c r="AB53" s="4"/>
+      <c r="AC53" s="4"/>
+      <c r="AD53" s="5"/>
+      <c r="AE53" s="5"/>
+      <c r="AF53" s="4"/>
+      <c r="AG53" s="4"/>
+      <c r="AH53" s="4"/>
+      <c r="AI53" s="4"/>
+      <c r="AJ53" s="4"/>
+      <c r="AK53" s="5"/>
+      <c r="AL53" s="5"/>
+      <c r="AM53" s="4"/>
+      <c r="AN53" s="4"/>
+      <c r="AO53" s="4"/>
+      <c r="AP53" s="4"/>
+      <c r="AQ53" s="4"/>
+      <c r="AR53" s="7"/>
+      <c r="AS53" s="5"/>
+      <c r="AT53" s="4"/>
+      <c r="AU53" s="4"/>
+      <c r="AV53" s="4"/>
+      <c r="AW53" s="4"/>
+      <c r="AX53" s="4"/>
+      <c r="AY53" s="5"/>
+      <c r="AZ53" s="5"/>
+      <c r="BA53" s="4"/>
+      <c r="BB53" s="4"/>
+      <c r="BC53" s="4"/>
+      <c r="BD53" s="4"/>
+      <c r="BE53" s="4"/>
+      <c r="BF53" s="5"/>
+      <c r="BG53" s="5"/>
+      <c r="BH53" s="4"/>
+      <c r="BI53" s="4"/>
+      <c r="BJ53" s="18"/>
+      <c r="BK53" s="18"/>
+      <c r="BL53" s="18"/>
+      <c r="BM53" s="18"/>
+      <c r="BN53" s="5"/>
+      <c r="BO53" s="4"/>
+      <c r="BP53" s="4"/>
+      <c r="BQ53" s="4"/>
+      <c r="BR53" s="4"/>
+      <c r="BS53" s="4"/>
+      <c r="BT53" s="5"/>
+      <c r="BU53" s="5"/>
+      <c r="BV53" s="6"/>
+    </row>
+    <row r="54" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="4"/>
+      <c r="Z54" s="4"/>
+      <c r="AA54" s="4"/>
+      <c r="AB54" s="4"/>
+      <c r="AC54" s="4"/>
+      <c r="AD54" s="5"/>
+      <c r="AE54" s="5"/>
+      <c r="AF54" s="4"/>
+      <c r="AG54" s="4"/>
+      <c r="AH54" s="4"/>
+      <c r="AI54" s="4"/>
+      <c r="AJ54" s="4"/>
+      <c r="AK54" s="5"/>
+      <c r="AL54" s="5"/>
+      <c r="AM54" s="4"/>
+      <c r="AN54" s="4"/>
+      <c r="AO54" s="4"/>
+      <c r="AP54" s="4"/>
+      <c r="AQ54" s="4"/>
+      <c r="AR54" s="7"/>
+      <c r="AS54" s="5"/>
+      <c r="AT54" s="4"/>
+      <c r="AU54" s="4"/>
+      <c r="AV54" s="4"/>
+      <c r="AW54" s="4"/>
+      <c r="AX54" s="4"/>
+      <c r="AY54" s="5"/>
+      <c r="AZ54" s="5"/>
+      <c r="BA54" s="4"/>
+      <c r="BB54" s="4"/>
+      <c r="BC54" s="4"/>
+      <c r="BD54" s="4"/>
+      <c r="BE54" s="4"/>
+      <c r="BF54" s="5"/>
+      <c r="BG54" s="5"/>
+      <c r="BH54" s="4"/>
+      <c r="BI54" s="4"/>
+      <c r="BJ54" s="4"/>
+      <c r="BK54" s="4"/>
+      <c r="BL54" s="4"/>
+      <c r="BM54" s="5"/>
+      <c r="BN54" s="5"/>
+      <c r="BO54" s="4"/>
+      <c r="BP54" s="4"/>
+      <c r="BQ54" s="4"/>
+      <c r="BR54" s="4"/>
+      <c r="BS54" s="4"/>
+      <c r="BT54" s="5"/>
+      <c r="BU54" s="5"/>
+      <c r="BV54" s="6"/>
+    </row>
+    <row r="55" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="4">
+        <v>4</v>
+      </c>
+      <c r="E55" s="14">
+        <v>45824</v>
+      </c>
+      <c r="F55" s="14">
+        <v>45827</v>
+      </c>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="4"/>
+      <c r="V55" s="4"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="4"/>
+      <c r="Z55" s="4"/>
+      <c r="AA55" s="4"/>
+      <c r="AB55" s="4"/>
+      <c r="AC55" s="4"/>
+      <c r="AD55" s="5"/>
+      <c r="AE55" s="5"/>
+      <c r="AF55" s="4"/>
+      <c r="AG55" s="4"/>
+      <c r="AH55" s="4"/>
+      <c r="AI55" s="4"/>
+      <c r="AJ55" s="4"/>
+      <c r="AK55" s="5"/>
+      <c r="AL55" s="5"/>
+      <c r="AM55" s="4"/>
+      <c r="AN55" s="4"/>
+      <c r="AO55" s="4"/>
+      <c r="AP55" s="4"/>
+      <c r="AQ55" s="4"/>
+      <c r="AR55" s="7"/>
+      <c r="AS55" s="5"/>
+      <c r="AT55" s="4"/>
+      <c r="AU55" s="4"/>
+      <c r="AV55" s="4"/>
+      <c r="AW55" s="4"/>
+      <c r="AX55" s="4"/>
+      <c r="AY55" s="5"/>
+      <c r="AZ55" s="5"/>
+      <c r="BA55" s="4"/>
+      <c r="BB55" s="4"/>
+      <c r="BC55" s="4"/>
+      <c r="BD55" s="4"/>
+      <c r="BE55" s="4"/>
+      <c r="BG55" s="28"/>
+      <c r="BH55" s="19"/>
+      <c r="BI55" s="19"/>
+      <c r="BJ55" s="19"/>
+      <c r="BK55" s="19"/>
+      <c r="BL55" s="4"/>
+      <c r="BM55" s="5"/>
+      <c r="BN55" s="5"/>
+      <c r="BO55" s="4"/>
+      <c r="BP55" s="4"/>
+      <c r="BQ55" s="4"/>
+      <c r="BR55" s="4"/>
+      <c r="BS55" s="4"/>
+      <c r="BT55" s="5"/>
+      <c r="BU55" s="5"/>
+      <c r="BV55" s="6"/>
+    </row>
+    <row r="56" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="4">
+        <v>4</v>
+      </c>
+      <c r="E56" s="14">
+        <v>45825</v>
+      </c>
+      <c r="F56" s="14">
+        <v>45828</v>
+      </c>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="5"/>
+      <c r="X56" s="5"/>
+      <c r="Y56" s="4"/>
+      <c r="Z56" s="4"/>
+      <c r="AA56" s="4"/>
+      <c r="AB56" s="4"/>
+      <c r="AC56" s="4"/>
+      <c r="AD56" s="5"/>
+      <c r="AE56" s="5"/>
+      <c r="AF56" s="4"/>
+      <c r="AG56" s="4"/>
+      <c r="AH56" s="4"/>
+      <c r="AI56" s="4"/>
+      <c r="AJ56" s="4"/>
+      <c r="AK56" s="5"/>
+      <c r="AL56" s="5"/>
+      <c r="AM56" s="4"/>
+      <c r="AN56" s="4"/>
+      <c r="AO56" s="4"/>
+      <c r="AP56" s="4"/>
+      <c r="AQ56" s="4"/>
+      <c r="AR56" s="7"/>
+      <c r="AS56" s="5"/>
+      <c r="AT56" s="4"/>
+      <c r="AU56" s="4"/>
+      <c r="AV56" s="4"/>
+      <c r="AW56" s="4"/>
+      <c r="AX56" s="4"/>
+      <c r="AY56" s="5"/>
+      <c r="AZ56" s="5"/>
+      <c r="BA56" s="4"/>
+      <c r="BB56" s="4"/>
+      <c r="BC56" s="4"/>
+      <c r="BD56" s="4"/>
+      <c r="BE56" s="4"/>
+      <c r="BF56" s="5"/>
+      <c r="BG56" s="5"/>
+      <c r="BH56" s="27"/>
+      <c r="BI56" s="18"/>
+      <c r="BJ56" s="18"/>
+      <c r="BK56" s="18"/>
+      <c r="BL56" s="18"/>
+      <c r="BM56" s="5"/>
+      <c r="BN56" s="5"/>
+      <c r="BO56" s="4"/>
+      <c r="BP56" s="4"/>
+      <c r="BQ56" s="4"/>
+      <c r="BR56" s="4"/>
+      <c r="BS56" s="4"/>
+      <c r="BT56" s="5"/>
+      <c r="BU56" s="5"/>
+      <c r="BV56" s="6"/>
+    </row>
+    <row r="57" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D57" s="4">
+        <v>4</v>
+      </c>
+      <c r="E57" s="14">
+        <v>45826</v>
+      </c>
+      <c r="F57" s="14">
+        <v>45829</v>
+      </c>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+      <c r="V57" s="4"/>
+      <c r="W57" s="5"/>
+      <c r="X57" s="5"/>
+      <c r="Y57" s="4"/>
+      <c r="Z57" s="4"/>
+      <c r="AA57" s="4"/>
+      <c r="AB57" s="4"/>
+      <c r="AC57" s="4"/>
+      <c r="AD57" s="5"/>
+      <c r="AE57" s="5"/>
+      <c r="AF57" s="4"/>
+      <c r="AG57" s="4"/>
+      <c r="AH57" s="4"/>
+      <c r="AI57" s="4"/>
+      <c r="AJ57" s="4"/>
+      <c r="AK57" s="5"/>
+      <c r="AL57" s="5"/>
+      <c r="AM57" s="4"/>
+      <c r="AN57" s="4"/>
+      <c r="AO57" s="4"/>
+      <c r="AP57" s="4"/>
+      <c r="AQ57" s="4"/>
+      <c r="AR57" s="7"/>
+      <c r="AS57" s="5"/>
+      <c r="AT57" s="4"/>
+      <c r="AU57" s="4"/>
+      <c r="AV57" s="4"/>
+      <c r="AW57" s="4"/>
+      <c r="AX57" s="4"/>
+      <c r="AY57" s="5"/>
+      <c r="AZ57" s="5"/>
+      <c r="BA57" s="4"/>
+      <c r="BB57" s="4"/>
+      <c r="BC57" s="4"/>
+      <c r="BD57" s="4"/>
+      <c r="BE57" s="4"/>
+      <c r="BF57" s="5"/>
+      <c r="BG57" s="5"/>
+      <c r="BH57" s="4"/>
+      <c r="BI57" s="4"/>
+      <c r="BJ57" s="18"/>
+      <c r="BK57" s="18"/>
+      <c r="BL57" s="18"/>
+      <c r="BM57" s="18"/>
+      <c r="BN57" s="5"/>
+      <c r="BO57" s="4"/>
+      <c r="BP57" s="4"/>
+      <c r="BQ57" s="4"/>
+      <c r="BR57" s="4"/>
+      <c r="BS57" s="4"/>
+      <c r="BT57" s="5"/>
+      <c r="BU57" s="5"/>
+      <c r="BV57" s="6"/>
+    </row>
+    <row r="58" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" s="4">
+        <v>1</v>
+      </c>
+      <c r="E58" s="14">
+        <v>45829</v>
+      </c>
+      <c r="F58" s="14">
+        <v>45829</v>
+      </c>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="4"/>
+      <c r="V58" s="4"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="5"/>
+      <c r="Y58" s="4"/>
+      <c r="Z58" s="4"/>
+      <c r="AA58" s="4"/>
+      <c r="AB58" s="4"/>
+      <c r="AC58" s="4"/>
+      <c r="AD58" s="5"/>
+      <c r="AE58" s="5"/>
+      <c r="AF58" s="4"/>
+      <c r="AG58" s="4"/>
+      <c r="AH58" s="4"/>
+      <c r="AI58" s="4"/>
+      <c r="AJ58" s="4"/>
+      <c r="AK58" s="5"/>
+      <c r="AL58" s="5"/>
+      <c r="AM58" s="4"/>
+      <c r="AN58" s="4"/>
+      <c r="AO58" s="4"/>
+      <c r="AP58" s="4"/>
+      <c r="AQ58" s="4"/>
+      <c r="AR58" s="7"/>
+      <c r="AS58" s="5"/>
+      <c r="AT58" s="4"/>
+      <c r="AU58" s="4"/>
+      <c r="AV58" s="4"/>
+      <c r="AW58" s="4"/>
+      <c r="AX58" s="4"/>
+      <c r="AY58" s="5"/>
+      <c r="AZ58" s="5"/>
+      <c r="BA58" s="4"/>
+      <c r="BB58" s="4"/>
+      <c r="BC58" s="4"/>
+      <c r="BD58" s="4"/>
+      <c r="BE58" s="4"/>
+      <c r="BF58" s="5"/>
+      <c r="BG58" s="5"/>
+      <c r="BH58" s="4"/>
+      <c r="BI58" s="4"/>
+      <c r="BJ58" s="4"/>
+      <c r="BK58" s="4"/>
+      <c r="BL58" s="27"/>
+      <c r="BM58" s="18"/>
+      <c r="BN58" s="5"/>
+      <c r="BO58" s="4"/>
+      <c r="BP58" s="4"/>
+      <c r="BQ58" s="4"/>
+      <c r="BR58" s="4"/>
+      <c r="BS58" s="4"/>
+      <c r="BT58" s="5"/>
+      <c r="BU58" s="5"/>
+      <c r="BV58" s="6"/>
+    </row>
+    <row r="59" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="4"/>
+      <c r="U59" s="4"/>
+      <c r="V59" s="4"/>
+      <c r="W59" s="5"/>
+      <c r="X59" s="5"/>
+      <c r="Y59" s="4"/>
+      <c r="Z59" s="4"/>
+      <c r="AA59" s="4"/>
+      <c r="AB59" s="4"/>
+      <c r="AC59" s="4"/>
+      <c r="AD59" s="5"/>
+      <c r="AE59" s="5"/>
+      <c r="AF59" s="4"/>
+      <c r="AG59" s="4"/>
+      <c r="AH59" s="4"/>
+      <c r="AI59" s="4"/>
+      <c r="AJ59" s="4"/>
+      <c r="AK59" s="5"/>
+      <c r="AL59" s="5"/>
+      <c r="AM59" s="4"/>
+      <c r="AN59" s="4"/>
+      <c r="AO59" s="4"/>
+      <c r="AP59" s="4"/>
+      <c r="AQ59" s="4"/>
+      <c r="AR59" s="7"/>
+      <c r="AS59" s="5"/>
+      <c r="AT59" s="4"/>
+      <c r="AU59" s="4"/>
+      <c r="AV59" s="4"/>
+      <c r="AW59" s="4"/>
+      <c r="AX59" s="4"/>
+      <c r="AY59" s="5"/>
+      <c r="AZ59" s="5"/>
+      <c r="BA59" s="4"/>
+      <c r="BB59" s="4"/>
+      <c r="BC59" s="4"/>
+      <c r="BD59" s="4"/>
+      <c r="BE59" s="4"/>
+      <c r="BF59" s="5"/>
+      <c r="BG59" s="5"/>
+      <c r="BH59" s="4"/>
+      <c r="BI59" s="4"/>
+      <c r="BJ59" s="4"/>
+      <c r="BK59" s="4"/>
+      <c r="BL59" s="4"/>
+      <c r="BM59" s="5"/>
+      <c r="BN59" s="5"/>
+      <c r="BO59" s="4"/>
+      <c r="BP59" s="4"/>
+      <c r="BQ59" s="4"/>
+      <c r="BR59" s="4"/>
+      <c r="BS59" s="4"/>
+      <c r="BT59" s="5"/>
+      <c r="BU59" s="5"/>
+      <c r="BV59" s="6"/>
+    </row>
+    <row r="60" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="4">
+        <v>2</v>
+      </c>
+      <c r="E60" s="14">
+        <v>45829</v>
+      </c>
+      <c r="F60" s="14">
+        <v>45830</v>
+      </c>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="4"/>
+      <c r="V60" s="4"/>
+      <c r="W60" s="5"/>
+      <c r="X60" s="5"/>
+      <c r="Y60" s="4"/>
+      <c r="Z60" s="4"/>
+      <c r="AA60" s="4"/>
+      <c r="AB60" s="4"/>
+      <c r="AC60" s="4"/>
+      <c r="AD60" s="5"/>
+      <c r="AE60" s="5"/>
+      <c r="AF60" s="4"/>
+      <c r="AG60" s="4"/>
+      <c r="AH60" s="4"/>
+      <c r="AI60" s="4"/>
+      <c r="AJ60" s="4"/>
+      <c r="AK60" s="5"/>
+      <c r="AL60" s="5"/>
+      <c r="AM60" s="4"/>
+      <c r="AN60" s="4"/>
+      <c r="AO60" s="4"/>
+      <c r="AP60" s="4"/>
+      <c r="AQ60" s="4"/>
+      <c r="AR60" s="7"/>
+      <c r="AS60" s="5"/>
+      <c r="AT60" s="4"/>
+      <c r="AU60" s="4"/>
+      <c r="AV60" s="4"/>
+      <c r="AW60" s="4"/>
+      <c r="AX60" s="4"/>
+      <c r="AY60" s="5"/>
+      <c r="AZ60" s="5"/>
+      <c r="BA60" s="4"/>
+      <c r="BB60" s="4"/>
+      <c r="BC60" s="4"/>
+      <c r="BD60" s="4"/>
+      <c r="BE60" s="4"/>
+      <c r="BF60" s="5"/>
+      <c r="BG60" s="5"/>
+      <c r="BH60" s="4"/>
+      <c r="BI60" s="4"/>
+      <c r="BJ60" s="4"/>
+      <c r="BK60" s="4"/>
+      <c r="BL60" s="27"/>
+      <c r="BM60" s="18"/>
+      <c r="BN60" s="18"/>
+      <c r="BO60" s="4"/>
+      <c r="BP60" s="4"/>
+      <c r="BQ60" s="4"/>
+      <c r="BR60" s="4"/>
+      <c r="BS60" s="4"/>
+      <c r="BT60" s="5"/>
+      <c r="BU60" s="5"/>
+      <c r="BV60" s="6"/>
+    </row>
+    <row r="61" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+      <c r="U61" s="4"/>
+      <c r="V61" s="4"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="4"/>
+      <c r="Z61" s="4"/>
+      <c r="AA61" s="4"/>
+      <c r="AB61" s="4"/>
+      <c r="AC61" s="4"/>
+      <c r="AD61" s="5"/>
+      <c r="AE61" s="5"/>
+      <c r="AF61" s="4"/>
+      <c r="AG61" s="4"/>
+      <c r="AH61" s="4"/>
+      <c r="AI61" s="4"/>
+      <c r="AJ61" s="4"/>
+      <c r="AK61" s="5"/>
+      <c r="AL61" s="5"/>
+      <c r="AM61" s="4"/>
+      <c r="AN61" s="4"/>
+      <c r="AO61" s="4"/>
+      <c r="AP61" s="4"/>
+      <c r="AQ61" s="4"/>
+      <c r="AR61" s="7"/>
+      <c r="AS61" s="5"/>
+      <c r="AT61" s="4"/>
+      <c r="AU61" s="4"/>
+      <c r="AV61" s="4"/>
+      <c r="AW61" s="4"/>
+      <c r="AX61" s="4"/>
+      <c r="AY61" s="5"/>
+      <c r="AZ61" s="5"/>
+      <c r="BA61" s="4"/>
+      <c r="BB61" s="4"/>
+      <c r="BC61" s="4"/>
+      <c r="BD61" s="4"/>
+      <c r="BE61" s="4"/>
+      <c r="BF61" s="5"/>
+      <c r="BG61" s="5"/>
+      <c r="BH61" s="4"/>
+      <c r="BI61" s="4"/>
+      <c r="BJ61" s="4"/>
+      <c r="BK61" s="4"/>
+      <c r="BL61" s="4"/>
+      <c r="BM61" s="5"/>
+      <c r="BN61" s="5"/>
+      <c r="BO61" s="4"/>
+      <c r="BP61" s="4"/>
+      <c r="BQ61" s="4"/>
+      <c r="BR61" s="4"/>
+      <c r="BS61" s="4"/>
+      <c r="BT61" s="5"/>
+      <c r="BU61" s="5"/>
+      <c r="BV61" s="6"/>
+    </row>
+    <row r="62" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="4">
+        <v>3</v>
+      </c>
+      <c r="E62" s="14">
+        <v>45828</v>
+      </c>
+      <c r="F62" s="14">
+        <v>45830</v>
+      </c>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="5"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="4"/>
+      <c r="V62" s="4"/>
+      <c r="W62" s="5"/>
+      <c r="X62" s="5"/>
+      <c r="Y62" s="4"/>
+      <c r="Z62" s="4"/>
+      <c r="AA62" s="4"/>
+      <c r="AB62" s="4"/>
+      <c r="AC62" s="4"/>
+      <c r="AD62" s="5"/>
+      <c r="AE62" s="5"/>
+      <c r="AF62" s="4"/>
+      <c r="AG62" s="4"/>
+      <c r="AH62" s="4"/>
+      <c r="AI62" s="4"/>
+      <c r="AJ62" s="4"/>
+      <c r="AK62" s="5"/>
+      <c r="AL62" s="5"/>
+      <c r="AM62" s="4"/>
+      <c r="AN62" s="4"/>
+      <c r="AO62" s="4"/>
+      <c r="AP62" s="4"/>
+      <c r="AQ62" s="4"/>
+      <c r="AR62" s="7"/>
+      <c r="AS62" s="5"/>
+      <c r="AT62" s="4"/>
+      <c r="AU62" s="4"/>
+      <c r="AV62" s="4"/>
+      <c r="AW62" s="4"/>
+      <c r="AX62" s="4"/>
+      <c r="AY62" s="5"/>
+      <c r="AZ62" s="5"/>
+      <c r="BA62" s="4"/>
+      <c r="BB62" s="4"/>
+      <c r="BC62" s="4"/>
+      <c r="BD62" s="4"/>
+      <c r="BE62" s="4"/>
+      <c r="BF62" s="5"/>
+      <c r="BG62" s="5"/>
+      <c r="BH62" s="4"/>
+      <c r="BI62" s="4"/>
+      <c r="BJ62" s="4"/>
+      <c r="BK62" s="4"/>
+      <c r="BL62" s="18"/>
+      <c r="BM62" s="18"/>
+      <c r="BN62" s="18"/>
+      <c r="BO62" s="4"/>
+      <c r="BP62" s="4"/>
+      <c r="BQ62" s="4"/>
+      <c r="BR62" s="4"/>
+      <c r="BS62" s="4"/>
+      <c r="BT62" s="5"/>
+      <c r="BU62" s="5"/>
+      <c r="BV62" s="6"/>
+    </row>
+    <row r="63" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4"/>
+      <c r="P63" s="5"/>
+      <c r="Q63" s="5"/>
+      <c r="R63" s="4"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
+      <c r="U63" s="4"/>
+      <c r="V63" s="4"/>
+      <c r="W63" s="5"/>
+      <c r="X63" s="5"/>
+      <c r="Y63" s="4"/>
+      <c r="Z63" s="4"/>
+      <c r="AA63" s="4"/>
+      <c r="AB63" s="4"/>
+      <c r="AC63" s="4"/>
+      <c r="AD63" s="5"/>
+      <c r="AE63" s="5"/>
+      <c r="AF63" s="4"/>
+      <c r="AG63" s="4"/>
+      <c r="AH63" s="4"/>
+      <c r="AI63" s="4"/>
+      <c r="AJ63" s="4"/>
+      <c r="AK63" s="5"/>
+      <c r="AL63" s="5"/>
+      <c r="AM63" s="4"/>
+      <c r="AN63" s="4"/>
+      <c r="AO63" s="4"/>
+      <c r="AP63" s="4"/>
+      <c r="AQ63" s="4"/>
+      <c r="AR63" s="7"/>
+      <c r="AS63" s="5"/>
+      <c r="AT63" s="4"/>
+      <c r="AU63" s="4"/>
+      <c r="AV63" s="4"/>
+      <c r="AW63" s="4"/>
+      <c r="AX63" s="4"/>
+      <c r="AY63" s="5"/>
+      <c r="AZ63" s="5"/>
+      <c r="BA63" s="4"/>
+      <c r="BB63" s="4"/>
+      <c r="BC63" s="4"/>
+      <c r="BD63" s="4"/>
+      <c r="BE63" s="4"/>
+      <c r="BF63" s="5"/>
+      <c r="BG63" s="5"/>
+      <c r="BH63" s="4"/>
+      <c r="BI63" s="4"/>
+      <c r="BJ63" s="4"/>
+      <c r="BK63" s="4"/>
+      <c r="BL63" s="4"/>
+      <c r="BM63" s="5"/>
+      <c r="BN63" s="5"/>
+      <c r="BO63" s="4"/>
+      <c r="BP63" s="4"/>
+      <c r="BQ63" s="4"/>
+      <c r="BR63" s="4"/>
+      <c r="BS63" s="4"/>
+      <c r="BT63" s="5"/>
+      <c r="BU63" s="5"/>
+      <c r="BV63" s="6"/>
+    </row>
+    <row r="64" spans="1:74" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
+      <c r="B64" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="10">
+        <v>3</v>
+      </c>
+      <c r="E64" s="15">
+        <v>45829</v>
+      </c>
+      <c r="F64" s="15">
+        <v>45831</v>
+      </c>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+      <c r="M64" s="12"/>
+      <c r="N64" s="10"/>
+      <c r="O64" s="10"/>
+      <c r="P64" s="11"/>
+      <c r="Q64" s="11"/>
+      <c r="R64" s="10"/>
+      <c r="S64" s="10"/>
+      <c r="T64" s="10"/>
+      <c r="U64" s="10"/>
+      <c r="V64" s="10"/>
+      <c r="W64" s="11"/>
+      <c r="X64" s="11"/>
+      <c r="Y64" s="10"/>
+      <c r="Z64" s="10"/>
+      <c r="AA64" s="10"/>
+      <c r="AB64" s="10"/>
+      <c r="AC64" s="10"/>
+      <c r="AD64" s="11"/>
+      <c r="AE64" s="11"/>
+      <c r="AF64" s="10"/>
+      <c r="AG64" s="10"/>
+      <c r="AH64" s="10"/>
+      <c r="AI64" s="10"/>
+      <c r="AJ64" s="10"/>
+      <c r="AK64" s="11"/>
+      <c r="AL64" s="11"/>
+      <c r="AM64" s="10"/>
+      <c r="AN64" s="10"/>
+      <c r="AO64" s="10"/>
+      <c r="AP64" s="10"/>
+      <c r="AQ64" s="10"/>
+      <c r="AR64" s="13"/>
+      <c r="AS64" s="11"/>
+      <c r="AT64" s="10"/>
+      <c r="AU64" s="10"/>
+      <c r="AV64" s="10"/>
+      <c r="AW64" s="10"/>
+      <c r="AX64" s="10"/>
+      <c r="AY64" s="11"/>
+      <c r="AZ64" s="11"/>
+      <c r="BA64" s="10"/>
+      <c r="BB64" s="10"/>
+      <c r="BC64" s="10"/>
+      <c r="BD64" s="10"/>
+      <c r="BE64" s="10"/>
+      <c r="BF64" s="11"/>
+      <c r="BG64" s="11"/>
+      <c r="BH64" s="10"/>
+      <c r="BI64" s="10"/>
+      <c r="BJ64" s="10"/>
+      <c r="BK64" s="10"/>
+      <c r="BL64" s="29"/>
+      <c r="BM64" s="20"/>
+      <c r="BN64" s="20"/>
+      <c r="BO64" s="20"/>
+      <c r="BP64" s="10"/>
+      <c r="BQ64" s="10"/>
+      <c r="BR64" s="10"/>
+      <c r="BS64" s="10"/>
+      <c r="BT64" s="11"/>
+      <c r="BU64" s="11"/>
+      <c r="BV64" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="G1:M1"/>
+  <mergeCells count="28">
     <mergeCell ref="N1:AR1"/>
     <mergeCell ref="AS1:BV1"/>
     <mergeCell ref="BW1:DA1"/>
     <mergeCell ref="DB1:EF1"/>
+    <mergeCell ref="YE1:ZF1"/>
+    <mergeCell ref="ZG1:AAK1"/>
+    <mergeCell ref="AAL1:ABI1"/>
+    <mergeCell ref="PX1:RB1"/>
+    <mergeCell ref="RC1:SG1"/>
+    <mergeCell ref="SH1:TK1"/>
+    <mergeCell ref="TL1:UP1"/>
+    <mergeCell ref="UQ1:VT1"/>
+    <mergeCell ref="G39:M39"/>
+    <mergeCell ref="N39:AR39"/>
+    <mergeCell ref="AS39:BV39"/>
+    <mergeCell ref="VU1:WY1"/>
+    <mergeCell ref="WZ1:YD1"/>
+    <mergeCell ref="KD1:LE1"/>
+    <mergeCell ref="LF1:MJ1"/>
+    <mergeCell ref="MK1:NN1"/>
+    <mergeCell ref="NO1:OS1"/>
+    <mergeCell ref="OT1:PW1"/>
     <mergeCell ref="EG1:FJ1"/>
     <mergeCell ref="FK1:GO1"/>
     <mergeCell ref="GP1:HS1"/>
     <mergeCell ref="HT1:IX1"/>
     <mergeCell ref="IY1:KC1"/>
-    <mergeCell ref="KD1:LE1"/>
-    <mergeCell ref="LF1:MJ1"/>
-    <mergeCell ref="MK1:NN1"/>
-    <mergeCell ref="NO1:OS1"/>
-    <mergeCell ref="OT1:PW1"/>
-    <mergeCell ref="PX1:RB1"/>
-    <mergeCell ref="RC1:SG1"/>
-    <mergeCell ref="SH1:TK1"/>
-    <mergeCell ref="TL1:UP1"/>
-    <mergeCell ref="UQ1:VT1"/>
-    <mergeCell ref="VU1:WY1"/>
-    <mergeCell ref="WZ1:YD1"/>
-    <mergeCell ref="YE1:ZF1"/>
-    <mergeCell ref="ZG1:AAK1"/>
-    <mergeCell ref="AAL1:ABI1"/>
+    <mergeCell ref="G1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>